<commit_message>
Mofidy Transport accounting template
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -281,15 +281,6 @@
     <t>JOB NO</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>MaKH</t>
-  </si>
-  <si>
-    <t>Loai DV</t>
-  </si>
-  <si>
     <t xml:space="preserve">SỐ CONT  
 </t>
   </si>
@@ -298,9 +289,6 @@
   </si>
   <si>
     <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN THÁNG 1 (TRANSPORTATION)</t>
-  </si>
-  <si>
-    <t>Accounting nhập?</t>
   </si>
   <si>
     <t>có VAT</t>
@@ -390,7 +378,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,8 +706,17 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,14 +845,8 @@
         <fgColor indexed="26"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1066,6 +1057,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1136,7 +1138,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1194,9 +1196,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1249,14 +1248,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1277,10 +1270,22 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1305,19 +1310,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="26" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="26" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1329,23 +1334,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1364,6 +1357,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1877,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1909,7 +1908,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75">
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="51" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2004,91 +2003,91 @@
       <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
+      <c r="A6" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="74"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
     </row>
     <row r="9" spans="1:19" ht="15.75">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
       <c r="S9" s="29"/>
     </row>
     <row r="10" spans="1:19" s="4" customFormat="1" ht="15.75">
@@ -2097,7 +2096,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D10" s="31"/>
       <c r="F10" s="11"/>
@@ -2121,7 +2120,7 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D11" s="31"/>
       <c r="F11" s="12"/>
@@ -2145,7 +2144,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D12" s="31"/>
       <c r="F12" s="12"/>
@@ -2169,17 +2168,17 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="31"/>
       <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="66"/>
+      <c r="G13" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="67"/>
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -2194,9 +2193,9 @@
     </row>
     <row r="14" spans="1:19" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="59"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -2209,75 +2208,73 @@
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64" t="s">
-        <v>70</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
       <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="80"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="86" t="s">
+      <c r="G15" s="81"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="82" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="67" t="s">
+      <c r="J15" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" s="67" t="s">
+      <c r="L15" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="84" t="s">
+      <c r="N15" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="84" t="s">
+      <c r="O15" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="77" t="s">
+      <c r="P15" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="67" t="s">
+      <c r="Q15" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="67" t="s">
+      <c r="R15" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="67" t="s">
+      <c r="S15" s="68" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="68"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
       <c r="F16" s="32" t="s">
         <v>21</v>
       </c>
@@ -2287,241 +2284,241 @@
       <c r="H16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="87"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="68"/>
-      <c r="R16" s="68"/>
-      <c r="S16" s="68"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
+      <c r="P16" s="79"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="69"/>
     </row>
     <row r="17" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="92">
+        <v>22700000</v>
+      </c>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+    </row>
+    <row r="18" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="35">
-        <v>22700000</v>
-      </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="62"/>
-    </row>
-    <row r="18" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="C18" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="E18" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="G18" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="H18" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="I18" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="J18" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="K18" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="L18" s="91" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="M18" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="N18" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="O18" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="L18" s="33" t="s">
+      <c r="P18" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="M18" s="33" t="s">
+      <c r="Q18" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="N18" s="33" t="s">
+      <c r="R18" s="91" t="s">
         <v>92</v>
       </c>
-      <c r="O18" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="P18" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q18" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="R18" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="S18" s="33"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62"/>
+      <c r="S18" s="91"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
     </row>
     <row r="19" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A19" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="62"/>
-      <c r="U19" s="62"/>
-    </row>
-    <row r="20" spans="1:21" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A20" s="69" t="s">
+      <c r="A19" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="92"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="60"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+    </row>
+    <row r="20" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="59"/>
+    </row>
+    <row r="21" spans="1:21" s="6" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A21" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="36">
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="35">
         <f>SUM(G17:G19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="50">
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="49">
         <f>SUM(K17:K19)</f>
         <v>22700000</v>
       </c>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="39"/>
-    </row>
-    <row r="21" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-    </row>
-    <row r="22" spans="1:21" s="6" customFormat="1" ht="18.75">
-      <c r="A22" s="21" t="s">
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="38"/>
+    </row>
+    <row r="22" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A22" s="11"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" s="6" customFormat="1" ht="18.75">
+      <c r="A23" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="71">
-        <f>S20</f>
+      <c r="K23" s="72">
+        <f>S21</f>
         <v>0</v>
       </c>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="72"/>
-    </row>
-    <row r="23" spans="1:21" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="72"/>
+      <c r="S23" s="73"/>
+    </row>
+    <row r="24" spans="1:21" s="6" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="S23" s="40"/>
-    </row>
-    <row r="24" spans="1:21" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
-    <row r="25" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1"/>
-    <row r="26" spans="1:21" s="6" customFormat="1" ht="15.75">
-      <c r="A26" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-    </row>
+      <c r="S24" s="39"/>
+    </row>
+    <row r="25" spans="1:21" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
+    <row r="26" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1"/>
     <row r="27" spans="1:21" s="6" customFormat="1" ht="15.75">
       <c r="A27" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2531,10 +2528,20 @@
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
     </row>
     <row r="28" spans="1:21" s="6" customFormat="1" ht="15.75">
       <c r="A28" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -2547,59 +2554,61 @@
     </row>
     <row r="29" spans="1:21" s="6" customFormat="1" ht="15.75">
       <c r="A29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
+        <v>12</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75">
-      <c r="A31" s="26" t="s">
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:21" s="6" customFormat="1" ht="15.75">
+      <c r="A30" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.75">
+      <c r="A32" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
-      <c r="A32" s="26"/>
-    </row>
-    <row r="33" spans="1:16" ht="18.75">
-      <c r="C33" s="60" t="str">
+    <row r="33" spans="1:16" ht="15.75">
+      <c r="A33" s="26"/>
+    </row>
+    <row r="34" spans="1:16" ht="18.75">
+      <c r="C34" s="57" t="str">
         <f>S1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="G33" s="27"/>
-      <c r="K33" s="2" t="s">
+      <c r="E34" s="2"/>
+      <c r="G34" s="27"/>
+      <c r="K34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2" t="s">
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
-      <c r="A38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
     <row r="39" spans="1:16">
-      <c r="B39" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="5:5">
-      <c r="E57" s="30"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="58" spans="5:5">
+      <c r="E58" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2611,8 +2620,8 @@
     <mergeCell ref="M15:M16"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="S15:S16"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K22:S22"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="K23:S23"/>
     <mergeCell ref="A6:S7"/>
     <mergeCell ref="A8:S8"/>
     <mergeCell ref="A15:A16"/>
@@ -2661,7 +2670,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75">
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="54" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2732,67 +2741,67 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="90"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
     </row>
     <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
     </row>
     <row r="9" spans="1:13" ht="15.75">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="29" t="s">
         <v>52</v>
       </c>
@@ -2873,8 +2882,8 @@
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2887,47 +2896,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="92" t="s">
+      <c r="D15" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="92" t="s">
+      <c r="F15" s="81"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="92" t="s">
+      <c r="I15" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="67" t="s">
+      <c r="K15" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="67" t="s">
+      <c r="M15" s="68" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="93"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="93"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="90"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2937,150 +2946,150 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A17" s="42">
+      <c r="A17" s="41">
         <v>1</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="43">
         <v>42012</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="42">
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="41">
         <v>1</v>
       </c>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="46">
         <v>1600000</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="46">
         <f>I17*1.1</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="K17" s="47"/>
-      <c r="L17" s="48">
+      <c r="K17" s="46"/>
+      <c r="L17" s="47">
         <f>J17+K17</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="89"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="86"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A18" s="42">
+      <c r="A18" s="41">
         <v>2</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="43">
         <v>42023</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="44">
         <v>1</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="55" t="s">
+      <c r="F18" s="44"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="46">
         <v>5000000</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="46">
         <f t="shared" ref="J18:J19" si="0">I18*1.1</f>
         <v>5500000</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="46">
         <v>550000</v>
       </c>
-      <c r="L18" s="48">
+      <c r="L18" s="47">
         <f>J18+K18</f>
         <v>6050000</v>
       </c>
-      <c r="M18" s="46" t="s">
+      <c r="M18" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="88"/>
-      <c r="O18" s="89"/>
+      <c r="N18" s="85"/>
+      <c r="O18" s="86"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A19" s="42">
+      <c r="A19" s="41">
         <v>3</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="43">
         <v>42033</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="42">
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="41">
         <v>1</v>
       </c>
-      <c r="H19" s="55" t="s">
+      <c r="H19" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="46">
         <v>1600000</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="46">
         <f t="shared" si="0"/>
         <v>1760000.0000000002</v>
       </c>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48">
+      <c r="K19" s="46"/>
+      <c r="L19" s="47">
         <f>J19+K19</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="89"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="86"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="51">
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="50">
         <f>SUM(E17:E19)</f>
         <v>1</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="50">
         <f>SUM(F17:F19)</f>
         <v>0</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="49">
+      <c r="I20" s="48">
         <f>SUM(I17:I19)</f>
         <v>8200000</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J20" s="48">
         <f>SUM(J17:J19)</f>
         <v>9020000</v>
       </c>
@@ -3122,11 +3131,11 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="73"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>

</xml_diff>

<commit_message>
Update accounting transport report
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -288,12 +288,6 @@
     <t>VOLUMN</t>
   </si>
   <si>
-    <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN THÁNG 1 (TRANSPORTATION)</t>
-  </si>
-  <si>
-    <t>có VAT</t>
-  </si>
-  <si>
     <t>${custName}</t>
   </si>
   <si>
@@ -367,6 +361,9 @@
   </si>
   <si>
     <t>${item.otherfee}</t>
+  </si>
+  <si>
+    <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN THÁNG ${month} (TRANSPORTATION)</t>
   </si>
 </sst>
 </file>
@@ -1286,15 +1283,33 @@
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1319,12 +1334,6 @@
     <xf numFmtId="0" fontId="44" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1334,12 +1343,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1357,12 +1360,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1878,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:S19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2003,71 +2000,71 @@
       <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
+      <c r="A6" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="80"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
     </row>
     <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="52"/>
@@ -2096,7 +2093,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="31"/>
       <c r="F10" s="11"/>
@@ -2120,7 +2117,7 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="31"/>
       <c r="F11" s="12"/>
@@ -2144,7 +2141,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="31"/>
       <c r="F12" s="12"/>
@@ -2168,17 +2165,17 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="31"/>
       <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="67"/>
+      <c r="G13" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="75"/>
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -2207,74 +2204,72 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
-      <c r="P14" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="P14" s="12"/>
       <c r="Q14" s="65"/>
       <c r="R14" s="65"/>
       <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="78" t="s">
+      <c r="E15" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="80" t="s">
+      <c r="F15" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="81"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="83" t="s">
+      <c r="G15" s="85"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="83" t="s">
+      <c r="J15" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="68" t="s">
+      <c r="K15" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="68" t="s">
+      <c r="L15" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="68" t="s">
+      <c r="M15" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="78" t="s">
+      <c r="N15" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="78" t="s">
+      <c r="O15" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="78" t="s">
+      <c r="P15" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="68" t="s">
+      <c r="Q15" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="68" t="s">
+      <c r="R15" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="68" t="s">
+      <c r="S15" s="69" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="69"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="32" t="s">
         <v>21</v>
       </c>
@@ -2284,40 +2279,40 @@
       <c r="H16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="69"/>
-      <c r="R16" s="69"/>
-      <c r="S16" s="69"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
     </row>
     <row r="17" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="A17" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
+        <v>71</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="33"/>
-      <c r="F17" s="91"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
       <c r="J17" s="33"/>
-      <c r="K17" s="92">
+      <c r="K17" s="68">
         <v>22700000</v>
       </c>
-      <c r="L17" s="92"/>
-      <c r="M17" s="92"/>
-      <c r="N17" s="92"/>
-      <c r="O17" s="92"/>
-      <c r="P17" s="92"/>
-      <c r="Q17" s="92"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="68"/>
+      <c r="Q17" s="68"/>
       <c r="R17" s="33"/>
       <c r="S17" s="60"/>
       <c r="T17" s="59"/>
@@ -2325,83 +2320,83 @@
     </row>
     <row r="18" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="A18" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="91" t="s">
+      <c r="C18" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="91" t="s">
+      <c r="E18" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="91" t="s">
+      <c r="F18" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="91" t="s">
+      <c r="G18" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="91" t="s">
+      <c r="H18" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="91" t="s">
+      <c r="I18" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="91" t="s">
+      <c r="J18" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="91" t="s">
+      <c r="K18" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="91" t="s">
+      <c r="M18" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="K18" s="91" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="91" t="s">
+      <c r="N18" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="M18" s="91" t="s">
+      <c r="O18" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="N18" s="91" t="s">
+      <c r="P18" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="91" t="s">
+      <c r="Q18" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="P18" s="91" t="s">
+      <c r="R18" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="Q18" s="91" t="s">
-        <v>91</v>
-      </c>
-      <c r="R18" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="S18" s="91"/>
+      <c r="S18" s="67"/>
       <c r="T18" s="59"/>
       <c r="U18" s="59"/>
     </row>
     <row r="19" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
       <c r="A19" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
+        <v>72</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="33"/>
-      <c r="F19" s="91"/>
+      <c r="F19" s="67"/>
       <c r="G19" s="33"/>
       <c r="H19" s="33"/>
       <c r="I19" s="33"/>
       <c r="J19" s="33"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="92"/>
-      <c r="M19" s="92"/>
-      <c r="N19" s="92"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="92"/>
-      <c r="Q19" s="92"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="68"/>
+      <c r="P19" s="68"/>
+      <c r="Q19" s="68"/>
       <c r="R19" s="33"/>
       <c r="S19" s="60"/>
       <c r="T19" s="59"/>
@@ -2431,14 +2426,14 @@
       <c r="U20" s="59"/>
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
       <c r="G21" s="35">
         <f>SUM(G17:G19)</f>
         <v>0</v>
@@ -2495,18 +2490,18 @@
       <c r="J23" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K23" s="72">
+      <c r="K23" s="78">
         <f>S21</f>
         <v>0</v>
       </c>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="72"/>
-      <c r="Q23" s="72"/>
-      <c r="R23" s="72"/>
-      <c r="S23" s="73"/>
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="78"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="79"/>
     </row>
     <row r="24" spans="1:21" s="6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A24" s="6" t="s">
@@ -2612,12 +2607,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="M15:M16"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="S15:S16"/>
     <mergeCell ref="A21:F21"/>
@@ -2634,6 +2623,12 @@
     <mergeCell ref="Q15:Q16"/>
     <mergeCell ref="R15:R16"/>
     <mergeCell ref="N15:N16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="M15:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2741,53 +2736,53 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
     </row>
     <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
     </row>
     <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="55"/>
@@ -2896,47 +2891,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="89" t="s">
+      <c r="F15" s="85"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="89" t="s">
+      <c r="I15" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="68" t="s">
+      <c r="J15" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="68" t="s">
+      <c r="K15" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="68" t="s">
+      <c r="L15" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="68" t="s">
+      <c r="M15" s="69" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="90"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="90"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2946,12 +2941,12 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A17" s="41">
@@ -2987,8 +2982,8 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M17" s="45"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="86"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="88"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A18" s="41">
@@ -3028,8 +3023,8 @@
       <c r="M18" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="85"/>
-      <c r="O18" s="86"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="88"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A19" s="41">
@@ -3065,16 +3060,16 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M19" s="45"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="86"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="88"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
       <c r="E20" s="50">
         <f>SUM(E17:E19)</f>
         <v>1</v>
@@ -3131,11 +3126,11 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="73"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>

</xml_diff>

<commit_message>
- Add to local
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -281,15 +281,6 @@
     <t>JOB NO</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>MaKH</t>
-  </si>
-  <si>
-    <t>Loai DV</t>
-  </si>
-  <si>
     <t xml:space="preserve">SỐ CONT  
 </t>
   </si>
@@ -297,15 +288,6 @@
     <t>VOLUMN</t>
   </si>
   <si>
-    <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN THÁNG 1 (TRANSPORTATION)</t>
-  </si>
-  <si>
-    <t>Accounting nhập?</t>
-  </si>
-  <si>
-    <t>có VAT</t>
-  </si>
-  <si>
     <t>${custName}</t>
   </si>
   <si>
@@ -379,6 +361,9 @@
   </si>
   <si>
     <t>${item.otherfee}</t>
+  </si>
+  <si>
+    <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN THÁNG ${month} (TRANSPORTATION)</t>
   </si>
 </sst>
 </file>
@@ -390,7 +375,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,8 +703,17 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,14 +842,8 @@
         <fgColor indexed="26"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1066,6 +1054,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1136,7 +1135,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1194,9 +1193,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1249,14 +1245,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1277,19 +1267,49 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1305,19 +1325,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="26" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="26" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1327,24 +1341,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1877,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1909,7 +1905,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75">
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="51" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2004,91 +2000,91 @@
       <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
+      <c r="A6" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="80"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="74"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
     </row>
     <row r="9" spans="1:19" ht="15.75">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
       <c r="S9" s="29"/>
     </row>
     <row r="10" spans="1:19" s="4" customFormat="1" ht="15.75">
@@ -2097,7 +2093,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="31" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D10" s="31"/>
       <c r="F10" s="11"/>
@@ -2121,7 +2117,7 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="31" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D11" s="31"/>
       <c r="F11" s="12"/>
@@ -2145,7 +2141,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="31" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D12" s="31"/>
       <c r="F12" s="12"/>
@@ -2169,17 +2165,17 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="31"/>
       <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="66"/>
+      <c r="G13" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="75"/>
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -2194,9 +2190,9 @@
     </row>
     <row r="14" spans="1:19" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="59"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -2208,76 +2204,72 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
-      <c r="P14" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64" t="s">
-        <v>70</v>
-      </c>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
       <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="80"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="86" t="s">
+      <c r="G15" s="85"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="82" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="67" t="s">
+      <c r="J15" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" s="67" t="s">
+      <c r="L15" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="84" t="s">
+      <c r="N15" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="84" t="s">
+      <c r="O15" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="77" t="s">
+      <c r="P15" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="67" t="s">
+      <c r="Q15" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="67" t="s">
+      <c r="R15" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="67" t="s">
+      <c r="S15" s="69" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="68"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="32" t="s">
         <v>21</v>
       </c>
@@ -2287,241 +2279,241 @@
       <c r="H16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="87"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="68"/>
-      <c r="R16" s="68"/>
-      <c r="S16" s="68"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
     </row>
     <row r="17" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="68">
+        <v>22700000</v>
+      </c>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="68"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+    </row>
+    <row r="18" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="35">
-        <v>22700000</v>
-      </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="62"/>
-    </row>
-    <row r="18" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="E18" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="G18" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="I18" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="J18" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="K18" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="M18" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="N18" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="O18" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="P18" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="Q18" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="L18" s="33" t="s">
+      <c r="R18" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="M18" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="N18" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="O18" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="P18" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q18" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="R18" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="S18" s="33"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62"/>
+      <c r="S18" s="67"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
     </row>
     <row r="19" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A19" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="62"/>
-      <c r="U19" s="62"/>
-    </row>
-    <row r="20" spans="1:21" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A20" s="69" t="s">
+      <c r="A19" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="68"/>
+      <c r="P19" s="68"/>
+      <c r="Q19" s="68"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="60"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+    </row>
+    <row r="20" spans="1:21" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="59"/>
+    </row>
+    <row r="21" spans="1:21" s="6" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A21" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="36">
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="35">
         <f>SUM(G17:G19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="50">
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="49">
         <f>SUM(K17:K19)</f>
         <v>22700000</v>
       </c>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="39"/>
-    </row>
-    <row r="21" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-    </row>
-    <row r="22" spans="1:21" s="6" customFormat="1" ht="18.75">
-      <c r="A22" s="21" t="s">
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="38"/>
+    </row>
+    <row r="22" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A22" s="11"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" s="6" customFormat="1" ht="18.75">
+      <c r="A23" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="71">
-        <f>S20</f>
+      <c r="K23" s="78">
+        <f>S21</f>
         <v>0</v>
       </c>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="72"/>
-    </row>
-    <row r="23" spans="1:21" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="78"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="79"/>
+    </row>
+    <row r="24" spans="1:21" s="6" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="S23" s="40"/>
-    </row>
-    <row r="24" spans="1:21" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
-    <row r="25" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1"/>
-    <row r="26" spans="1:21" s="6" customFormat="1" ht="15.75">
-      <c r="A26" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-    </row>
+      <c r="S24" s="39"/>
+    </row>
+    <row r="25" spans="1:21" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
+    <row r="26" spans="1:21" s="6" customFormat="1" ht="7.5" customHeight="1"/>
     <row r="27" spans="1:21" s="6" customFormat="1" ht="15.75">
       <c r="A27" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2531,10 +2523,20 @@
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
     </row>
     <row r="28" spans="1:21" s="6" customFormat="1" ht="15.75">
       <c r="A28" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -2547,72 +2549,68 @@
     </row>
     <row r="29" spans="1:21" s="6" customFormat="1" ht="15.75">
       <c r="A29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
+        <v>12</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75">
-      <c r="A31" s="26" t="s">
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:21" s="6" customFormat="1" ht="15.75">
+      <c r="A30" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.75">
+      <c r="A32" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
-      <c r="A32" s="26"/>
-    </row>
-    <row r="33" spans="1:16" ht="18.75">
-      <c r="C33" s="60" t="str">
+    <row r="33" spans="1:16" ht="15.75">
+      <c r="A33" s="26"/>
+    </row>
+    <row r="34" spans="1:16" ht="18.75">
+      <c r="C34" s="57" t="str">
         <f>S1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="G33" s="27"/>
-      <c r="K33" s="2" t="s">
+      <c r="E34" s="2"/>
+      <c r="G34" s="27"/>
+      <c r="K34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2" t="s">
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
-      <c r="A38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
     <row r="39" spans="1:16">
-      <c r="B39" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="5:5">
-      <c r="E57" s="30"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="58" spans="5:5">
+      <c r="E58" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="M15:M16"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="S15:S16"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K22:S22"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="K23:S23"/>
     <mergeCell ref="A6:S7"/>
     <mergeCell ref="A8:S8"/>
     <mergeCell ref="A15:A16"/>
@@ -2625,6 +2623,12 @@
     <mergeCell ref="Q15:Q16"/>
     <mergeCell ref="R15:R16"/>
     <mergeCell ref="N15:N16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="M15:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2661,7 +2665,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75">
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="54" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2732,67 +2736,67 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="90"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
     </row>
     <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
     </row>
     <row r="9" spans="1:13" ht="15.75">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="29" t="s">
         <v>52</v>
       </c>
@@ -2873,8 +2877,8 @@
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2887,47 +2891,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="92" t="s">
+      <c r="D15" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="92" t="s">
+      <c r="F15" s="85"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="92" t="s">
+      <c r="I15" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="67" t="s">
+      <c r="K15" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="67" t="s">
+      <c r="M15" s="69" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="93"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="93"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2937,150 +2941,150 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A17" s="42">
+      <c r="A17" s="41">
         <v>1</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="43">
         <v>42012</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="42">
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="41">
         <v>1</v>
       </c>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="46">
         <v>1600000</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="46">
         <f>I17*1.1</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="K17" s="47"/>
-      <c r="L17" s="48">
+      <c r="K17" s="46"/>
+      <c r="L17" s="47">
         <f>J17+K17</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="89"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="88"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A18" s="42">
+      <c r="A18" s="41">
         <v>2</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="43">
         <v>42023</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="44">
         <v>1</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="55" t="s">
+      <c r="F18" s="44"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="46">
         <v>5000000</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="46">
         <f t="shared" ref="J18:J19" si="0">I18*1.1</f>
         <v>5500000</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="46">
         <v>550000</v>
       </c>
-      <c r="L18" s="48">
+      <c r="L18" s="47">
         <f>J18+K18</f>
         <v>6050000</v>
       </c>
-      <c r="M18" s="46" t="s">
+      <c r="M18" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="88"/>
-      <c r="O18" s="89"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="88"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A19" s="42">
+      <c r="A19" s="41">
         <v>3</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="43">
         <v>42033</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="42">
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="41">
         <v>1</v>
       </c>
-      <c r="H19" s="55" t="s">
+      <c r="H19" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="46">
         <v>1600000</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="46">
         <f t="shared" si="0"/>
         <v>1760000.0000000002</v>
       </c>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48">
+      <c r="K19" s="46"/>
+      <c r="L19" s="47">
         <f>J19+K19</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="89"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="88"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="51">
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="50">
         <f>SUM(E17:E19)</f>
         <v>1</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="50">
         <f>SUM(F17:F19)</f>
         <v>0</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="49">
+      <c r="I20" s="48">
         <f>SUM(I17:I19)</f>
         <v>8200000</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J20" s="48">
         <f>SUM(J17:J19)</f>
         <v>9020000</v>
       </c>
@@ -3122,11 +3126,11 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="72"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>

</xml_diff>

<commit_message>
- All info for trans report
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -14,13 +14,14 @@
   <sheets>
     <sheet name="AGI- ND" sheetId="32" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="35" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -245,10 +246,6 @@
     <t>JOB NO</t>
   </si>
   <si>
-    <t xml:space="preserve">SỐ CONT  
-</t>
-  </si>
-  <si>
     <t>VOLUMN</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>${trans.noOfCont}</t>
   </si>
   <si>
-    <t>${trans.}</t>
-  </si>
-  <si>
     <t>${trans.volumn}</t>
   </si>
   <si>
@@ -325,17 +319,37 @@
   </si>
   <si>
     <t>${trans.otherfee}</t>
+  </si>
+  <si>
+    <t>${trans.total}</t>
+  </si>
+  <si>
+    <t>${chihoTotal}</t>
+  </si>
+  <si>
+    <t>${giacaTotal}</t>
+  </si>
+  <si>
+    <t>${otherTotal}</t>
+  </si>
+  <si>
+    <t>${total}</t>
+  </si>
+  <si>
+    <t>SỐ CONT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,24 +643,6 @@
       <sz val="14"/>
       <name val="Cordia New"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="26">
@@ -1060,7 +1056,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1127,12 +1123,6 @@
     <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1190,18 +1180,30 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1217,6 +1219,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1224,42 +1250,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1270,6 +1260,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1785,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1807,15 +1800,15 @@
     <col min="14" max="14" width="12.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" style="3" customWidth="1"/>
     <col min="16" max="16" width="12.42578125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="50.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="3" customWidth="1"/>
     <col min="19" max="19" width="16.7109375" style="3" customWidth="1"/>
     <col min="20" max="20" width="18" style="3" customWidth="1"/>
     <col min="21" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75">
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1910,91 +1903,91 @@
       <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1">
+      <c r="A7" s="73"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75">
+      <c r="A8" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-    </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1">
-      <c r="A7" s="72"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="72"/>
-      <c r="S7" s="72"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="73" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
     </row>
     <row r="9" spans="1:19" ht="15.75">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
       <c r="S9" s="29" t="s">
         <v>48</v>
       </c>
@@ -2005,7 +1998,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="31"/>
       <c r="F10" s="11"/>
@@ -2029,7 +2022,7 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="31"/>
       <c r="F11" s="12"/>
@@ -2053,7 +2046,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="31"/>
       <c r="F12" s="12"/>
@@ -2077,17 +2070,17 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="31"/>
       <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="67"/>
+      <c r="G13" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="69"/>
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -2102,15 +2095,15 @@
     </row>
     <row r="14" spans="1:19" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
-      <c r="B14" s="58"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="58"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="59"/>
+      <c r="J14" s="57"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -2122,66 +2115,66 @@
       <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="77"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="63" t="s">
+      <c r="G15" s="75"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="M15" s="65" t="s">
+      <c r="M15" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="61" t="s">
+      <c r="N15" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="61" t="s">
+      <c r="O15" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="61" t="s">
+      <c r="P15" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="81" t="s">
+      <c r="Q15" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="81" t="s">
+      <c r="R15" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="65" t="s">
+      <c r="S15" s="67" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="66"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
       <c r="F16" s="32" t="s">
         <v>21</v>
       </c>
@@ -2191,100 +2184,108 @@
       <c r="H16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="64"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="81"/>
-      <c r="S16" s="66"/>
-    </row>
-    <row r="17" spans="1:19" s="5" customFormat="1" ht="39.75" customHeight="1">
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="77"/>
+      <c r="R16" s="77"/>
+      <c r="S16" s="68"/>
+    </row>
+    <row r="17" spans="1:19" s="5" customFormat="1" ht="50.25" customHeight="1">
       <c r="A17" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="C17" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="D17" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="E17" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="F17" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="52" t="s">
+      <c r="G17" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="52" t="s">
+      <c r="H17" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="52" t="s">
+      <c r="I17" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="52" t="s">
+      <c r="J17" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="J17" s="52" t="s">
+      <c r="K17" s="50"/>
+      <c r="L17" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="52" t="s">
+      <c r="M17" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="52" t="s">
+      <c r="N17" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="M17" s="52" t="s">
+      <c r="O17" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="N17" s="52" t="s">
+      <c r="P17" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="O17" s="52" t="s">
+      <c r="Q17" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="52" t="s">
+      <c r="R17" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="Q17" s="52" t="s">
+      <c r="S17" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="R17" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
       <c r="J18" s="35"/>
-      <c r="K18" s="47" t="e">
+      <c r="K18" s="45" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="37"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q18" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="R18" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="S18" s="64" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="19" spans="1:19" s="6" customFormat="1" ht="7.5" customHeight="1">
       <c r="A19" s="11"/>
@@ -2322,21 +2323,23 @@
       <c r="J20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="70"/>
-      <c r="L20" s="70"/>
-      <c r="M20" s="70"/>
-      <c r="N20" s="70"/>
-      <c r="O20" s="70"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
-      <c r="S20" s="71"/>
+      <c r="K20" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="72"/>
+      <c r="Q20" s="72"/>
+      <c r="R20" s="72"/>
+      <c r="S20" s="72"/>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="S21" s="38"/>
+      <c r="S21" s="36"/>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
     <row r="23" spans="1:19" s="6" customFormat="1" ht="7.5" customHeight="1"/>
@@ -2411,7 +2414,7 @@
       <c r="A30" s="26"/>
     </row>
     <row r="31" spans="1:19" ht="18.75">
-      <c r="C31" s="56" t="str">
+      <c r="C31" s="54" t="str">
         <f>S1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
       </c>
@@ -2493,7 +2496,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75">
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="51" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2564,67 +2567,67 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="84"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="84"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
     </row>
     <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="85"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="83"/>
     </row>
     <row r="9" spans="1:13" ht="15.75">
-      <c r="A9" s="54"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="29" t="s">
         <v>52</v>
       </c>
@@ -2705,8 +2708,8 @@
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2719,47 +2722,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="76" t="s">
+      <c r="E15" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="86" t="s">
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="86" t="s">
+      <c r="I15" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="65" t="s">
+      <c r="J15" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="65" t="s">
+      <c r="K15" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="65" t="s">
+      <c r="L15" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="65" t="s">
+      <c r="M15" s="67" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="87"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="87"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="85"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2769,150 +2772,150 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A17" s="39">
+      <c r="A17" s="37">
         <v>1</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="39">
         <v>42012</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="39">
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="37">
         <v>1</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="42">
         <v>1600000</v>
       </c>
-      <c r="J17" s="44">
+      <c r="J17" s="42">
         <f>I17*1.1</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="K17" s="44"/>
-      <c r="L17" s="45">
+      <c r="K17" s="42"/>
+      <c r="L17" s="43">
         <f>J17+K17</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="M17" s="43"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="83"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="78"/>
+      <c r="O17" s="79"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A18" s="39">
+      <c r="A18" s="37">
         <v>2</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="39">
         <v>42023</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="40">
         <v>1</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="51" t="s">
+      <c r="F18" s="40"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="42">
         <v>5000000</v>
       </c>
-      <c r="J18" s="44">
+      <c r="J18" s="42">
         <f t="shared" ref="J18:J19" si="0">I18*1.1</f>
         <v>5500000</v>
       </c>
-      <c r="K18" s="44">
+      <c r="K18" s="42">
         <v>550000</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="43">
         <f>J18+K18</f>
         <v>6050000</v>
       </c>
-      <c r="M18" s="43" t="s">
+      <c r="M18" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="82"/>
-      <c r="O18" s="83"/>
+      <c r="N18" s="78"/>
+      <c r="O18" s="79"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A19" s="39">
+      <c r="A19" s="37">
         <v>3</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="39">
         <v>42033</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="39">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="37">
         <v>1</v>
       </c>
-      <c r="H19" s="51" t="s">
+      <c r="H19" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="42">
         <v>1600000</v>
       </c>
-      <c r="J19" s="44">
+      <c r="J19" s="42">
         <f t="shared" si="0"/>
         <v>1760000.0000000002</v>
       </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="45">
+      <c r="K19" s="42"/>
+      <c r="L19" s="43">
         <f>J19+K19</f>
         <v>1760000.0000000002</v>
       </c>
-      <c r="M19" s="43"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="83"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="79"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="48">
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="46">
         <f>SUM(E17:E19)</f>
         <v>1</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F20" s="46">
         <f>SUM(F17:F19)</f>
         <v>0</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="46">
+      <c r="I20" s="44">
         <f>SUM(I17:I19)</f>
         <v>8200000</v>
       </c>
-      <c r="J20" s="46">
+      <c r="J20" s="44">
         <f>SUM(J17:J19)</f>
         <v>9020000</v>
       </c>
@@ -2954,11 +2957,11 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="71"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="81"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>
@@ -3060,4 +3063,18 @@
   <pageSetup scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Finish vantai report
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -349,7 +349,7 @@
     <numFmt numFmtId="165" formatCode="0;[Red]0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,6 +647,13 @@
     <font>
       <b/>
       <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1184,7 +1191,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1200,42 +1206,33 @@
     <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1248,6 +1245,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1272,7 +1272,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="43" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1790,7 +1797,7 @@
   <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1914,71 +1921,71 @@
       <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="68"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="74"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
     </row>
     <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="48"/>
@@ -2080,7 +2087,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="85" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="10"/>
@@ -2088,12 +2095,11 @@
       <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="69"/>
+      <c r="H13" s="86"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -2114,7 +2120,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="57"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -2126,66 +2132,66 @@
       <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="D15" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="67" t="s">
+      <c r="G15" s="72"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="67" t="s">
+      <c r="K15" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="M15" s="67" t="s">
+      <c r="M15" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="65" t="s">
+      <c r="N15" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="65" t="s">
+      <c r="O15" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="65" t="s">
+      <c r="P15" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="78" t="s">
+      <c r="Q15" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="78" t="s">
+      <c r="R15" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="67" t="s">
+      <c r="S15" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="68"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="32" t="s">
         <v>21</v>
       </c>
@@ -2195,17 +2201,17 @@
       <c r="H16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78"/>
-      <c r="S16" s="68"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="64"/>
     </row>
     <row r="17" spans="1:19" s="5" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="33" t="s">
@@ -2223,13 +2229,13 @@
       <c r="E17" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F17" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="60" t="s">
+      <c r="H17" s="59" t="s">
         <v>79</v>
       </c>
       <c r="I17" s="50" t="s">
@@ -2251,28 +2257,28 @@
       <c r="O17" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="P17" s="61" t="s">
+      <c r="P17" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="Q17" s="61" t="s">
+      <c r="Q17" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="R17" s="61" t="s">
+      <c r="R17" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="S17" s="61" t="s">
+      <c r="S17" s="60" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
@@ -2281,20 +2287,20 @@
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="62" t="s">
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="Q18" s="62" t="s">
+      <c r="Q18" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R18" s="63" t="s">
+      <c r="R18" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="S18" s="64" t="s">
+      <c r="S18" s="62" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2329,22 +2335,22 @@
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="87" t="s">
+      <c r="H20" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="I20" s="87"/>
+      <c r="I20" s="75"/>
       <c r="J20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="72"/>
-      <c r="Q20" s="72"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="72"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="6" t="s">
@@ -2450,6 +2456,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="L15:L16"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="S15:S16"/>
     <mergeCell ref="A18:F18"/>
@@ -2466,13 +2479,6 @@
     <mergeCell ref="Q15:Q16"/>
     <mergeCell ref="R15:R16"/>
     <mergeCell ref="N15:N16"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="L15:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2579,53 +2585,53 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
     </row>
     <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
     </row>
     <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="52"/>
@@ -2734,47 +2740,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="85" t="s">
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="67" t="s">
+      <c r="K15" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="67" t="s">
+      <c r="M15" s="63" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="86"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2784,12 +2790,12 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A17" s="37">
@@ -2825,8 +2831,8 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M17" s="41"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
+      <c r="N17" s="76"/>
+      <c r="O17" s="77"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A18" s="37">
@@ -2866,8 +2872,8 @@
       <c r="M18" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="79"/>
-      <c r="O18" s="80"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="77"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A19" s="37">
@@ -2903,16 +2909,16 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M19" s="41"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
+      <c r="N19" s="76"/>
+      <c r="O19" s="77"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="46">
         <f>SUM(E17:E19)</f>
         <v>1</v>
@@ -2969,11 +2975,11 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="82"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>

</xml_diff>

<commit_message>
CR Report DV VanTai (Month Year -> StartDate and EndDate)
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="11295" windowHeight="4815"/>
+    <workbookView xWindow="675" yWindow="3720" windowWidth="19140" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="AGI- ND" sheetId="32" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="35" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="144525" calcMode="manual"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -261,9 +257,6 @@
     <t>${custFax}</t>
   </si>
   <si>
-    <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN THÁNG ${month} (TRANSPORTATION)</t>
-  </si>
-  <si>
     <t>Ref: ${refNo}</t>
   </si>
   <si>
@@ -334,19 +327,35 @@
   </si>
   <si>
     <t>SỐ CONT</t>
+  </si>
+  <si>
+    <t>BẢNG KÊ  CƯỚC VẬN CHUYỂN (TRANSPORTATION)</t>
+  </si>
+  <si>
+    <t>Từ ngày</t>
+  </si>
+  <si>
+    <t>Tới ngày</t>
+  </si>
+  <si>
+    <t>${startDate}</t>
+  </si>
+  <si>
+    <t>${endDate}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0;[Red]0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +664,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="26">
@@ -1068,7 +1084,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1207,51 +1223,51 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1275,6 +1291,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1544,7 +1569,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1579,7 +1604,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1788,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1818,12 +1843,12 @@
     <col min="20" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75">
+    <row r="1" spans="1:19" ht="18.75">
       <c r="R1" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="18.75">
+    <row r="2" spans="1:19" ht="18.75">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1845,7 +1870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="18.75">
+    <row r="3" spans="1:19" ht="18.75">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1867,7 +1892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="18.75">
+    <row r="4" spans="1:19" s="3" customFormat="1" ht="18.75">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1889,7 +1914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" s="8"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -1909,145 +1934,150 @@
       <c r="Q5" s="28"/>
       <c r="R5" s="28"/>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="73" t="s">
+    <row r="6" spans="1:19" ht="15" customHeight="1">
+      <c r="A6" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+    </row>
+    <row r="7" spans="1:19" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+    </row>
+    <row r="8" spans="1:19" s="3" customFormat="1" ht="19.5">
+      <c r="A8" s="8"/>
+      <c r="B8" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="88"/>
+      <c r="E8" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="89"/>
+      <c r="G8" s="88" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="88"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="9"/>
+    </row>
+    <row r="9" spans="1:19" s="3" customFormat="1" ht="15.75">
+      <c r="A9" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75">
-      <c r="A8" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="29" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+    </row>
+    <row r="10" spans="1:19" s="3" customFormat="1" ht="15.75">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" ht="15.75">
-      <c r="A10" s="10" t="s">
+    <row r="11" spans="1:19" s="4" customFormat="1" ht="15.75">
+      <c r="A11" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="15.75">
-      <c r="A11" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-    </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" ht="15.75">
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+    </row>
+    <row r="12" spans="1:19" s="4" customFormat="1" ht="15.75">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="31"/>
       <c r="F12" s="12"/>
@@ -2064,24 +2094,20 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="15.75">
+    <row r="13" spans="1:19" s="4" customFormat="1" ht="15.75">
       <c r="A13" s="10" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="69"/>
+      <c r="C13" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -2091,17 +2117,24 @@
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
     </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" ht="15.75">
-      <c r="A14" s="14"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11"/>
+    <row r="14" spans="1:19" s="4" customFormat="1" ht="15.75">
+      <c r="A14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="64"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -2111,249 +2144,247 @@
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
     </row>
-    <row r="15" spans="1:18" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="67" t="s">
+    <row r="15" spans="1:19" s="4" customFormat="1" ht="15.75">
+      <c r="A15" s="14"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+    </row>
+    <row r="16" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B16" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C16" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="D16" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E16" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F16" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="67" t="s">
+      <c r="G16" s="75"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="67" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="67" t="s">
+      <c r="J16" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L16" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="65" t="s">
+      <c r="M16" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="N15" s="65" t="s">
+      <c r="N16" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="65" t="s">
+      <c r="O16" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="P15" s="78" t="s">
+      <c r="P16" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="Q15" s="78" t="s">
+      <c r="Q16" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="R15" s="67" t="s">
+      <c r="R16" s="65" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="68"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="32" t="s">
+    <row r="17" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A17" s="66"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G17" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H17" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="68"/>
-    </row>
-    <row r="17" spans="1:18" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A17" s="33" t="s">
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="77"/>
+      <c r="Q17" s="77"/>
+      <c r="R17" s="66"/>
+    </row>
+    <row r="18" spans="1:19" s="5" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="C18" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="D18" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="E18" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="F18" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="G18" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="57" t="s">
+      <c r="H18" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="I18" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="49" t="s">
+      <c r="J18" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="49" t="s">
+      <c r="K18" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="49" t="s">
+      <c r="L18" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="L17" s="49" t="s">
+      <c r="M18" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="M17" s="49" t="s">
+      <c r="N18" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="N17" s="49" t="s">
+      <c r="O18" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="O17" s="59" t="s">
+      <c r="P18" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="P17" s="59" t="s">
+      <c r="Q18" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="Q17" s="59" t="s">
+      <c r="R18" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="R17" s="59" t="s">
+    </row>
+    <row r="19" spans="1:19" s="6" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A19" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="60" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A18" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="60" t="s">
+      <c r="P19" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="P18" s="60" t="s">
+      <c r="Q19" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="Q18" s="62" t="s">
+      <c r="R19" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R18" s="61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-    </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="18.75">
-      <c r="A20" s="21" t="s">
+    </row>
+    <row r="20" spans="1:19" s="6" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A20" s="11"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+    </row>
+    <row r="21" spans="1:19" s="6" customFormat="1" ht="18.75">
+      <c r="A21" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="64"/>
-      <c r="J20" s="23" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="78"/>
+      <c r="J21" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="72"/>
-      <c r="Q20" s="72"/>
-      <c r="R20" s="72"/>
-    </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69"/>
+    </row>
+    <row r="22" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="R21" s="36"/>
-    </row>
-    <row r="22" spans="1:18" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
-    <row r="23" spans="1:18" s="6" customFormat="1" ht="7.5" customHeight="1"/>
-    <row r="24" spans="1:18" s="6" customFormat="1" ht="15.75">
-      <c r="A24" s="24" t="s">
+      <c r="R22" s="36"/>
+    </row>
+    <row r="23" spans="1:19" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
+    <row r="24" spans="1:19" s="6" customFormat="1" ht="7.5" customHeight="1"/>
+    <row r="25" spans="1:19" s="6" customFormat="1" ht="15.75">
+      <c r="A25" s="24" t="s">
         <v>10</v>
-      </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-    </row>
-    <row r="25" spans="1:18" s="6" customFormat="1" ht="15.75">
-      <c r="A25" s="24" t="s">
-        <v>11</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
@@ -2363,10 +2394,19 @@
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
-    </row>
-    <row r="26" spans="1:18" s="6" customFormat="1" ht="15.75">
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+    </row>
+    <row r="26" spans="1:19" s="6" customFormat="1" ht="15.75">
       <c r="A26" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -2377,72 +2417,89 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:18" s="6" customFormat="1" ht="15.75">
+    <row r="27" spans="1:19" s="6" customFormat="1" ht="15.75">
       <c r="A27" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
+        <v>12</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-    </row>
-    <row r="29" spans="1:18" ht="15.75">
-      <c r="A29" s="26" t="s">
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:19" s="6" customFormat="1" ht="15.75">
+      <c r="A28" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+    </row>
+    <row r="30" spans="1:19" s="3" customFormat="1" ht="15.75">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.75">
-      <c r="A30" s="26"/>
-    </row>
-    <row r="31" spans="1:18" ht="18.75">
-      <c r="C31" s="53" t="str">
+    <row r="31" spans="1:19" s="3" customFormat="1" ht="15.75">
+      <c r="A31" s="26"/>
+    </row>
+    <row r="32" spans="1:19" s="3" customFormat="1" ht="18.75">
+      <c r="C32" s="53" t="str">
         <f>R1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="G31" s="27"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2" t="s">
+      <c r="E32" s="2"/>
+      <c r="G32" s="27"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="7:7">
-      <c r="G36" s="2"/>
-    </row>
-    <row r="55" spans="5:5">
-      <c r="E55" s="30"/>
+    <row r="37" spans="1:19" s="3" customFormat="1">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="49" spans="1:19" s="3" customFormat="1"/>
+    <row r="56" spans="1:19" s="3" customFormat="1">
+      <c r="E56" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="K20:R20"/>
+  <mergeCells count="25">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K21:R21"/>
     <mergeCell ref="A6:R7"/>
-    <mergeCell ref="A8:R8"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="A9:R9"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="H21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2710,40 +2767,40 @@
       <c r="B15" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="65" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
       <c r="H15" s="85" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="67" t="s">
+      <c r="K15" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="67" t="s">
+      <c r="M15" s="65" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
       <c r="A16" s="86"/>
       <c r="B16" s="86"/>
-      <c r="C16" s="68"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="86"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
@@ -2756,10 +2813,10 @@
       </c>
       <c r="H16" s="86"/>
       <c r="I16" s="86"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A17" s="37">
@@ -2877,12 +2934,12 @@
       <c r="O19" s="80"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
       <c r="E20" s="45">
         <f>SUM(E17:E19)</f>
         <v>1</v>

</xml_diff>

<commit_message>
Them so tien bang chu Noi lay cont noi ha cont da test
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="675" yWindow="3720" windowWidth="19140" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14950" windowHeight="3230"/>
   </bookViews>
   <sheets>
     <sheet name="AGI- ND" sheetId="32" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="35" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -343,6 +347,9 @@
   <si>
     <t>${endDate}</t>
   </si>
+  <si>
+    <t>${totalText}</t>
+  </si>
 </sst>
 </file>
 
@@ -355,7 +362,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="46">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,6 +678,15 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="26">
@@ -1084,7 +1100,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1223,49 +1239,58 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1292,14 +1317,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1569,7 +1588,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1604,7 +1623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1813,42 +1832,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22:J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="3" customWidth="1"/>
     <col min="6" max="6" width="6" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" style="3" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="13.1796875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.7265625" style="3" customWidth="1"/>
     <col min="19" max="19" width="18" style="3" customWidth="1"/>
     <col min="20" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75">
+    <row r="1" spans="1:18" ht="18.5">
       <c r="R1" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75">
+    <row r="2" spans="1:18" ht="18.5">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1870,7 +1889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="18.75">
+    <row r="3" spans="1:18" ht="18.5">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1892,7 +1911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" ht="18.75">
+    <row r="4" spans="1:18" ht="18.5">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1914,7 +1933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5" s="8"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -1934,7 +1953,7 @@
       <c r="Q5" s="28"/>
       <c r="R5" s="28"/>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1">
+    <row r="6" spans="1:18" ht="15" customHeight="1">
       <c r="A6" s="70" t="s">
         <v>93</v>
       </c>
@@ -1956,7 +1975,7 @@
       <c r="Q6" s="70"/>
       <c r="R6" s="70"/>
     </row>
-    <row r="7" spans="1:19" s="3" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:18" ht="15" customHeight="1">
       <c r="A7" s="70"/>
       <c r="B7" s="70"/>
       <c r="C7" s="70"/>
@@ -1976,23 +1995,23 @@
       <c r="Q7" s="70"/>
       <c r="R7" s="70"/>
     </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" ht="19.5">
+    <row r="8" spans="1:18" ht="19.5">
       <c r="A8" s="8"/>
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="88"/>
-      <c r="E8" s="89" t="s">
+      <c r="D8" s="80"/>
+      <c r="E8" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="89"/>
-      <c r="G8" s="88" t="s">
+      <c r="F8" s="81"/>
+      <c r="G8" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="88"/>
+      <c r="H8" s="80"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -2004,7 +2023,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:19" s="3" customFormat="1" ht="15.75">
+    <row r="9" spans="1:18" ht="15.5">
       <c r="A9" s="71" t="s">
         <v>69</v>
       </c>
@@ -2026,7 +2045,7 @@
       <c r="Q9" s="71"/>
       <c r="R9" s="71"/>
     </row>
-    <row r="10" spans="1:19" s="3" customFormat="1" ht="15.75">
+    <row r="10" spans="1:18" ht="15.5">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -2048,7 +2067,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="4" customFormat="1" ht="15.75">
+    <row r="11" spans="1:18" s="4" customFormat="1" ht="15.5">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
@@ -2071,7 +2090,7 @@
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
     </row>
-    <row r="12" spans="1:19" s="4" customFormat="1" ht="15.75">
+    <row r="12" spans="1:18" s="4" customFormat="1" ht="15.5">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2113,7 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="1:19" s="4" customFormat="1" ht="15.75">
+    <row r="13" spans="1:18" s="4" customFormat="1" ht="15.5">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -2117,7 +2136,7 @@
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
     </row>
-    <row r="14" spans="1:19" s="4" customFormat="1" ht="15.75">
+    <row r="14" spans="1:18" s="4" customFormat="1" ht="15.5">
       <c r="A14" s="10" t="s">
         <v>33</v>
       </c>
@@ -2130,10 +2149,10 @@
       <c r="F14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="64"/>
+      <c r="H14" s="79"/>
       <c r="I14" s="11"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
@@ -2144,7 +2163,7 @@
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
     </row>
-    <row r="15" spans="1:19" s="4" customFormat="1" ht="15.75">
+    <row r="15" spans="1:18" s="4" customFormat="1" ht="15.5">
       <c r="A15" s="14"/>
       <c r="B15" s="55"/>
       <c r="C15" s="11"/>
@@ -2164,7 +2183,7 @@
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="1:19" s="5" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:18" s="5" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="65" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2235,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="5" customFormat="1" ht="24.75" customHeight="1">
+    <row r="17" spans="1:18" s="5" customFormat="1" ht="24.75" customHeight="1">
       <c r="A17" s="66"/>
       <c r="B17" s="73"/>
       <c r="C17" s="66"/>
@@ -2242,7 +2261,7 @@
       <c r="Q17" s="77"/>
       <c r="R17" s="66"/>
     </row>
-    <row r="18" spans="1:19" s="5" customFormat="1" ht="19.5" customHeight="1">
+    <row r="18" spans="1:18" s="5" customFormat="1" ht="19.5" customHeight="1">
       <c r="A18" s="33" t="s">
         <v>70</v>
       </c>
@@ -2298,7 +2317,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="6" customFormat="1" ht="19.5" customHeight="1">
+    <row r="19" spans="1:18" s="6" customFormat="1" ht="19.5" customHeight="1">
       <c r="A19" s="67" t="s">
         <v>8</v>
       </c>
@@ -2328,7 +2347,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="6" customFormat="1" ht="7.5" customHeight="1">
+    <row r="20" spans="1:18" s="6" customFormat="1" ht="7.5" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -2348,7 +2367,7 @@
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
     </row>
-    <row r="21" spans="1:19" s="6" customFormat="1" ht="18.75">
+    <row r="21" spans="1:18" s="6" customFormat="1" ht="18.5">
       <c r="A21" s="21" t="s">
         <v>1</v>
       </c>
@@ -2374,15 +2393,21 @@
       <c r="Q21" s="69"/>
       <c r="R21" s="69"/>
     </row>
-    <row r="22" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1">
+    <row r="22" spans="1:18" s="6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="G22" s="90" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
       <c r="R22" s="36"/>
     </row>
-    <row r="23" spans="1:19" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
-    <row r="24" spans="1:19" s="6" customFormat="1" ht="7.5" customHeight="1"/>
-    <row r="25" spans="1:19" s="6" customFormat="1" ht="15.75">
+    <row r="23" spans="1:18" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
+    <row r="24" spans="1:18" s="6" customFormat="1" ht="7.5" customHeight="1"/>
+    <row r="25" spans="1:18" s="6" customFormat="1" ht="15.5">
       <c r="A25" s="24" t="s">
         <v>10</v>
       </c>
@@ -2404,7 +2429,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
     </row>
-    <row r="26" spans="1:19" s="6" customFormat="1" ht="15.75">
+    <row r="26" spans="1:18" s="6" customFormat="1" ht="15.5">
       <c r="A26" s="24" t="s">
         <v>11</v>
       </c>
@@ -2417,7 +2442,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:19" s="6" customFormat="1" ht="15.75">
+    <row r="27" spans="1:18" s="6" customFormat="1" ht="15.5">
       <c r="A27" s="24" t="s">
         <v>12</v>
       </c>
@@ -2430,7 +2455,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:19" s="6" customFormat="1" ht="15.75">
+    <row r="28" spans="1:18" s="6" customFormat="1" ht="15.5">
       <c r="A28" s="24" t="s">
         <v>13</v>
       </c>
@@ -2443,15 +2468,15 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="30" spans="1:19" s="3" customFormat="1" ht="15.75">
+    <row r="30" spans="1:18" ht="15.5">
       <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="3" customFormat="1" ht="15.75">
+    <row r="31" spans="1:18" ht="15.5">
       <c r="A31" s="26"/>
     </row>
-    <row r="32" spans="1:19" s="3" customFormat="1" ht="18.75">
+    <row r="32" spans="1:18" ht="18.5">
       <c r="C32" s="53" t="str">
         <f>R1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
@@ -2466,15 +2491,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="3" customFormat="1">
+    <row r="37" spans="7:7">
       <c r="G37" s="2"/>
     </row>
-    <row r="49" spans="1:19" s="3" customFormat="1"/>
-    <row r="56" spans="1:19" s="3" customFormat="1">
+    <row r="56" spans="5:5">
       <c r="E56" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
@@ -2485,6 +2509,7 @@
     <mergeCell ref="L16:L17"/>
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G22:J22"/>
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="K21:R21"/>
@@ -2515,31 +2540,31 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="3" customWidth="1"/>
     <col min="2" max="2" width="8" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="3" customWidth="1"/>
     <col min="4" max="4" width="26" style="3" customWidth="1"/>
     <col min="5" max="6" width="5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" style="3" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" style="3" customWidth="1"/>
     <col min="12" max="12" width="13" style="3" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="23.54296875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="5.81640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.7265625" style="3" customWidth="1"/>
     <col min="16" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75">
+    <row r="1" spans="1:13" ht="18.5">
       <c r="M1" s="50" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75">
+    <row r="2" spans="1:13" ht="18.5">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2556,7 +2581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75">
+    <row r="3" spans="1:13" ht="18.5">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2573,7 +2598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.75">
+    <row r="4" spans="1:13" ht="18.5">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2606,55 +2631,55 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="84" t="s">
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.5">
+      <c r="A8" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75">
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.5">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -2671,7 +2696,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" ht="15.75">
+    <row r="10" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -2689,7 +2714,7 @@
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" ht="15.75">
+    <row r="11" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2707,7 +2732,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="15.75">
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -2725,7 +2750,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" ht="15.75">
+    <row r="13" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
@@ -2745,7 +2770,7 @@
       </c>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" ht="15.75">
+    <row r="14" spans="1:13" s="4" customFormat="1" ht="15.5">
       <c r="A14" s="14"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -2761,16 +2786,16 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="88" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="88" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="74" t="s">
@@ -2778,10 +2803,10 @@
       </c>
       <c r="F15" s="75"/>
       <c r="G15" s="76"/>
-      <c r="H15" s="85" t="s">
+      <c r="H15" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="88" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="65" t="s">
@@ -2797,11 +2822,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
+    <row r="16" spans="1:13" s="5" customFormat="1" ht="15.5">
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="66"/>
-      <c r="D16" s="86"/>
+      <c r="D16" s="89"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2811,8 +2836,8 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
       <c r="J16" s="66"/>
       <c r="K16" s="66"/>
       <c r="L16" s="66"/>
@@ -2852,8 +2877,8 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M17" s="41"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="83"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A18" s="37">
@@ -2893,8 +2918,8 @@
       <c r="M18" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="N18" s="79"/>
-      <c r="O18" s="80"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="83"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A19" s="37">
@@ -2930,8 +2955,8 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M19" s="41"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="83"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
       <c r="A20" s="67" t="s">
@@ -2968,7 +2993,7 @@
       </c>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="1:15" s="6" customFormat="1" ht="15.75">
+    <row r="21" spans="1:15" s="6" customFormat="1" ht="15.5">
       <c r="A21" s="11"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -2983,7 +3008,7 @@
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" ht="18.75">
+    <row r="22" spans="1:15" s="6" customFormat="1" ht="18.5">
       <c r="A22" s="21" t="s">
         <v>1</v>
       </c>
@@ -2996,17 +3021,17 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="82"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:15" s="6" customFormat="1" ht="15.75" hidden="1"/>
-    <row r="25" spans="1:15" s="6" customFormat="1" ht="15.75">
+    <row r="24" spans="1:15" s="6" customFormat="1" ht="15.5" hidden="1"/>
+    <row r="25" spans="1:15" s="6" customFormat="1" ht="15.5">
       <c r="A25" s="24" t="s">
         <v>10</v>
       </c>
@@ -3023,7 +3048,7 @@
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
     </row>
-    <row r="26" spans="1:15" s="6" customFormat="1" ht="15.75">
+    <row r="26" spans="1:15" s="6" customFormat="1" ht="15.5">
       <c r="A26" s="24" t="s">
         <v>11</v>
       </c>
@@ -3034,7 +3059,7 @@
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:15" s="6" customFormat="1" ht="15.75">
+    <row r="27" spans="1:15" s="6" customFormat="1" ht="15.5">
       <c r="A27" s="24" t="s">
         <v>12</v>
       </c>
@@ -3045,7 +3070,7 @@
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="1:15" s="6" customFormat="1" ht="15.75">
+    <row r="28" spans="1:15" s="6" customFormat="1" ht="15.5">
       <c r="A28" s="24" t="s">
         <v>13</v>
       </c>
@@ -3056,15 +3081,15 @@
       <c r="F28" s="22"/>
       <c r="G28" s="25"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75">
+    <row r="30" spans="1:15" ht="15.5">
       <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75">
+    <row r="31" spans="1:15" ht="15.5">
       <c r="A31" s="26"/>
     </row>
-    <row r="32" spans="1:15" ht="18.75">
+    <row r="32" spans="1:15" ht="18.5">
       <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
@@ -3112,7 +3137,7 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Fixed debit van tai
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14950" windowHeight="3230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="3225"/>
   </bookViews>
   <sheets>
     <sheet name="AGI- ND" sheetId="32" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -149,10 +149,6 @@
 (CÓ VAT)</t>
   </si>
   <si>
-    <t>PHÁT SINH KHÁC 
-(CÓ VAT)</t>
-  </si>
-  <si>
     <t>TEL</t>
   </si>
   <si>
@@ -312,9 +308,6 @@
     <t>${trans.accountingPrice}</t>
   </si>
   <si>
-    <t>${trans.otherfee}</t>
-  </si>
-  <si>
     <t>${trans.total}</t>
   </si>
   <si>
@@ -324,9 +317,6 @@
     <t>${giacaTotal}</t>
   </si>
   <si>
-    <t>${otherTotal}</t>
-  </si>
-  <si>
     <t>${total}</t>
   </si>
   <si>
@@ -349,6 +339,69 @@
   </si>
   <si>
     <t>${totalText}</t>
+  </si>
+  <si>
+    <t>${trans.vat}</t>
+  </si>
+  <si>
+    <t>TIỀN THUẾ</t>
+  </si>
+  <si>
+    <t>THUẾ GTGT</t>
+  </si>
+  <si>
+    <t>${trans.vatAmount}</t>
+  </si>
+  <si>
+    <t>GHI CHÚ</t>
+  </si>
+  <si>
+    <t>${trans.note}</t>
+  </si>
+  <si>
+    <t>${feeName}</t>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${feeVal.feeVal}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${feeNames}" var="feeName"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${trans.convertedFeeThu}" var="feeVal"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${tranreports}" var="trans"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${totaTruckingFees}" var="feeTotal"&gt;</t>
+  </si>
+  <si>
+    <t>${feeTotal}</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>${trans.noOfOthCont}</t>
+  </si>
+  <si>
+    <t>${vatAmountTotal}</t>
+  </si>
+  <si>
+    <t>THÀNH TIỀN</t>
+  </si>
+  <si>
+    <t>${trans.feeWithVat}</t>
+  </si>
+  <si>
+    <t>${finalTotal}</t>
+  </si>
+  <si>
+    <t>${thanhtien}</t>
   </si>
 </sst>
 </file>
@@ -362,7 +415,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="51">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,8 +749,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -824,6 +901,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1108,7 +1191,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1238,18 +1321,135 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="48" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="47" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="50" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="43" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="49" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="49" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1259,12 +1459,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1274,17 +1468,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1309,27 +1497,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="43" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1843,42 +2010,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="H21" activeCellId="8" sqref="R18 Q18 P18 O18 O19 P19 Q19 R19 H21:I21"/>
+    <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
+      <pane xSplit="10" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="6" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.453125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.1796875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.1796875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.453125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="16.7265625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="18" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="3"/>
+    <col min="7" max="8" width="6.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="3" customWidth="1"/>
+    <col min="18" max="24" width="14.42578125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="18" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.5">
-      <c r="R1" s="46" t="s">
+    <row r="1" spans="1:26" ht="18.75">
+      <c r="Y1" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="18.5">
+    <row r="2" spans="1:26" ht="18.75">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1886,7 +2055,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -1896,11 +2065,18 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="18.5">
+    <row r="3" spans="1:26" ht="18.75">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1908,7 +2084,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1918,11 +2094,18 @@
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="18.5">
+    <row r="4" spans="1:26" ht="18.75">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1930,7 +2113,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -1940,11 +2123,18 @@
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:26">
       <c r="A5" s="8"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -1963,67 +2153,88 @@
       <c r="P5" s="28"/>
       <c r="Q5" s="28"/>
       <c r="R5" s="28"/>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="66"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-    </row>
-    <row r="8" spans="1:18" ht="19.5">
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1">
+      <c r="A6" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
+      <c r="Q6" s="107"/>
+      <c r="R6" s="107"/>
+      <c r="S6" s="107"/>
+      <c r="T6" s="107"/>
+      <c r="U6" s="107"/>
+      <c r="V6" s="107"/>
+      <c r="W6" s="107"/>
+      <c r="X6" s="107"/>
+      <c r="Y6" s="107"/>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1">
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="107"/>
+      <c r="U7" s="107"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+    </row>
+    <row r="8" spans="1:26" ht="19.5">
       <c r="A8" s="8"/>
       <c r="B8" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="98"/>
+      <c r="E8" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="99"/>
+      <c r="G8" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="75" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="75"/>
-      <c r="E8" s="76" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" s="75"/>
-      <c r="I8" s="8"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -2032,31 +2243,45 @@
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="9"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.5">
-      <c r="A9" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="67"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.5">
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75">
+      <c r="A9" s="108" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108"/>
+      <c r="T9" s="108"/>
+      <c r="U9" s="108"/>
+      <c r="V9" s="108"/>
+      <c r="W9" s="108"/>
+      <c r="X9" s="108"/>
+      <c r="Y9" s="108"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -2064,35 +2289,42 @@
       <c r="E10" s="47"/>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="52"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="54"/>
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
       <c r="O10" s="52"/>
-      <c r="P10" s="47"/>
+      <c r="P10" s="52"/>
       <c r="Q10" s="47"/>
-      <c r="R10" s="29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="15.5">
+      <c r="R10" s="47"/>
+      <c r="S10" s="61"/>
+      <c r="T10" s="78"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="15.75">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="31"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="13"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -2100,21 +2332,28 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" ht="15.5">
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="15.75">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="31"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="11"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="12"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
@@ -2123,21 +2362,28 @@
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
-    </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="15.5">
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+    </row>
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="15.75">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="31"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="12"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
@@ -2146,26 +2392,33 @@
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
-    </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" ht="15.5">
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+    </row>
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="31"/>
       <c r="F14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="74"/>
-      <c r="I14" s="11"/>
-      <c r="K14" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="G14" s="102" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="11"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
@@ -2173,8 +2426,15 @@
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
-    </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" ht="15.5">
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+    </row>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="15.75">
       <c r="A15" s="14"/>
       <c r="B15" s="55"/>
       <c r="C15" s="11"/>
@@ -2182,9 +2442,9 @@
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="12"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
@@ -2193,273 +2453,394 @@
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
-    </row>
-    <row r="16" spans="1:18" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="61" t="s">
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+    </row>
+    <row r="16" spans="1:26" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="100" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="95" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="100" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="109" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="95" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="L16" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="68" t="s">
+      <c r="M16" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="71"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="J16" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" s="68" t="s">
+      <c r="O16" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="68" t="s">
+      <c r="P16" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="O16" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="P16" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q16" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16" s="61" t="s">
+      <c r="R16" s="112" t="s">
+        <v>98</v>
+      </c>
+      <c r="S16" s="112" t="s">
+        <v>97</v>
+      </c>
+      <c r="T16" s="90" t="s">
+        <v>113</v>
+      </c>
+      <c r="U16" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="V16" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="W16" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="X16" s="94" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A17" s="62"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="Y16" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z16" s="89"/>
+    </row>
+    <row r="17" spans="1:26" s="5" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A17" s="96"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
       <c r="F17" s="32" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="62"/>
-    </row>
-    <row r="18" spans="1:18" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A18" s="33" t="s">
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="101"/>
+      <c r="O17" s="101"/>
+      <c r="P17" s="101"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112"/>
+      <c r="T17" s="91"/>
+      <c r="U17" s="92"/>
+      <c r="V17" s="93"/>
+      <c r="W17" s="94"/>
+      <c r="X17" s="94"/>
+      <c r="Y17" s="94"/>
+      <c r="Z17" s="89"/>
+    </row>
+    <row r="18" spans="1:26" s="5" customFormat="1" ht="15.75">
+      <c r="A18" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="64"/>
+      <c r="T18" s="76"/>
+      <c r="U18" s="73"/>
+      <c r="V18" s="64"/>
+      <c r="W18" s="64"/>
+      <c r="X18" s="64"/>
+      <c r="Y18" s="64"/>
+    </row>
+    <row r="19" spans="1:26" s="5" customFormat="1" ht="18" customHeight="1">
+      <c r="A19" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="C19" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="D19" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="E19" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="F19" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="G19" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="57" t="s">
+      <c r="H19" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="J19" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="49" t="s">
+      <c r="K19" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="49" t="s">
+      <c r="L19" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="49" t="s">
+      <c r="M19" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="L18" s="49" t="s">
+      <c r="N19" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="M18" s="49" t="s">
+      <c r="O19" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="N18" s="49" t="s">
+      <c r="P19" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="O18" s="87" t="s">
+      <c r="Q19" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="P18" s="87" t="s">
+      <c r="R19" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="S19" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="T19" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="U19" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="V19" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="W19" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="X19" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="Q18" s="87" t="s">
+      <c r="Y19" s="68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" s="5" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A20" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="71"/>
+      <c r="W20" s="72"/>
+      <c r="X20" s="62"/>
+      <c r="Y20" s="68"/>
+    </row>
+    <row r="21" spans="1:26" s="6" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A21" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="104"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="R18" s="87" t="s">
+      <c r="Q21" s="84" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A19" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="88" t="s">
+      <c r="R21" s="85"/>
+      <c r="S21" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="T21" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="U21" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="V21" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="W21" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="X21" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="P19" s="88" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q19" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="R19" s="90" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-    </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" ht="18.5">
-      <c r="A21" s="21" t="s">
+      <c r="Y21" s="69"/>
+    </row>
+    <row r="22" spans="1:26" s="6" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A22" s="11"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+    </row>
+    <row r="23" spans="1:26" s="6" customFormat="1" ht="18.75">
+      <c r="A23" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="91" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" s="91"/>
-      <c r="J21" s="23" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="113" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="113"/>
+      <c r="K23" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="65"/>
-      <c r="Q21" s="65"/>
-      <c r="R21" s="65"/>
-    </row>
-    <row r="22" spans="1:18" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A22" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="85"/>
-      <c r="C22" s="85"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="G22" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="R22" s="36"/>
-    </row>
-    <row r="23" spans="1:18" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
-    <row r="24" spans="1:18" s="6" customFormat="1" ht="7.5" customHeight="1"/>
-    <row r="25" spans="1:18" s="6" customFormat="1" ht="15.5">
-      <c r="A25" s="24" t="s">
+      <c r="L23" s="106"/>
+      <c r="M23" s="106"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="106"/>
+      <c r="Q23" s="106"/>
+      <c r="R23" s="106"/>
+      <c r="S23" s="106"/>
+      <c r="T23" s="106"/>
+      <c r="U23" s="106"/>
+      <c r="V23" s="106"/>
+      <c r="W23" s="106"/>
+      <c r="X23" s="106"/>
+      <c r="Y23" s="106"/>
+    </row>
+    <row r="24" spans="1:26" s="6" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A24" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="G24" s="105" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="105"/>
+      <c r="N24" s="105"/>
+      <c r="O24" s="105"/>
+      <c r="P24" s="105"/>
+      <c r="Q24" s="105"/>
+      <c r="R24" s="105"/>
+      <c r="S24" s="105"/>
+      <c r="T24" s="105"/>
+      <c r="V24" s="81"/>
+      <c r="Y24" s="36"/>
+    </row>
+    <row r="25" spans="1:26" s="6" customFormat="1" ht="7.5" hidden="1" customHeight="1"/>
+    <row r="26" spans="1:26" s="6" customFormat="1" ht="7.5" customHeight="1"/>
+    <row r="27" spans="1:26" s="6" customFormat="1" ht="15.75">
+      <c r="A27" s="24" t="s">
         <v>10</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-    </row>
-    <row r="26" spans="1:18" s="6" customFormat="1" ht="15.5">
-      <c r="A26" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-    </row>
-    <row r="27" spans="1:18" s="6" customFormat="1" ht="15.5">
-      <c r="A27" s="24" t="s">
-        <v>12</v>
       </c>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2469,78 +2850,113 @@
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
-    </row>
-    <row r="28" spans="1:18" s="6" customFormat="1" ht="15.5">
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+    </row>
+    <row r="28" spans="1:26" s="6" customFormat="1" ht="15.75">
       <c r="A28" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+        <v>11</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-    </row>
-    <row r="30" spans="1:18" ht="15.5">
-      <c r="A30" s="26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15.5">
-      <c r="A31" s="26"/>
-    </row>
-    <row r="32" spans="1:18" ht="18.5">
-      <c r="C32" s="53" t="str">
-        <f>R1</f>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="1:26" s="6" customFormat="1" ht="15.75">
+      <c r="A29" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75">
+      <c r="A30" s="26"/>
+    </row>
+    <row r="31" spans="1:26" ht="18.75">
+      <c r="C31" s="53" t="str">
+        <f>Y1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="G32" s="27"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2" t="s">
+      <c r="E31" s="2"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="7:7">
-      <c r="G37" s="2"/>
-    </row>
-    <row r="56" spans="5:5">
-      <c r="E56" s="30"/>
+    <row r="36" spans="7:8">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="A6:R7"/>
-    <mergeCell ref="A9:R9"/>
+  <mergeCells count="34">
+    <mergeCell ref="A6:Y7"/>
+    <mergeCell ref="A9:Y9"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="J16:J17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="M16:M17"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="G24:T24"/>
+    <mergeCell ref="L23:Y23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2556,31 +2972,31 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="8" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="26" style="3" customWidth="1"/>
     <col min="5" max="6" width="5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="3" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="3" customWidth="1"/>
     <col min="12" max="12" width="13" style="3" customWidth="1"/>
-    <col min="13" max="13" width="23.54296875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="5.81640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="3" customWidth="1"/>
     <col min="16" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.5">
+    <row r="1" spans="1:13" ht="18.75">
       <c r="M1" s="50" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.5">
+    <row r="2" spans="1:13" ht="18.75">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2597,7 +3013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.5">
+    <row r="3" spans="1:13" ht="18.75">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2614,7 +3030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.5">
+    <row r="4" spans="1:13" ht="18.75">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2647,55 +3063,55 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="118"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="81"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.5">
-      <c r="A8" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.5">
+      <c r="A7" s="118"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75">
+      <c r="A8" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -2709,10 +3125,10 @@
       <c r="K9" s="51"/>
       <c r="L9" s="51"/>
       <c r="M9" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" ht="15.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -2730,7 +3146,7 @@
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" ht="15.5">
+    <row r="11" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2748,7 +3164,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="15.5">
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -2766,15 +3182,15 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" ht="15.5">
+    <row r="13" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A13" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="31"/>
       <c r="E13" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="11"/>
@@ -2782,11 +3198,11 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" ht="15.5">
+    <row r="14" spans="1:13" s="4" customFormat="1" ht="15.75">
       <c r="A14" s="14"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -2802,47 +3218,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="95" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="109" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="110"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="120" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="71"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="83" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="83" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="61" t="s">
+      <c r="K15" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="61" t="s">
+      <c r="L15" s="95" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="15.5">
-      <c r="A16" s="84"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="84"/>
+      <c r="M15" s="95" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
+      <c r="A16" s="121"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="121"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -2852,25 +3268,25 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="96"/>
+      <c r="M16" s="96"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A17" s="37">
         <v>1</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="39">
         <v>42012</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
@@ -2878,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="42">
         <v>1600000</v>
@@ -2893,21 +3309,21 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M17" s="41"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="78"/>
+      <c r="N17" s="114"/>
+      <c r="O17" s="115"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A18" s="37">
         <v>2</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="39">
         <v>42023</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="40">
         <v>1</v>
@@ -2915,7 +3331,7 @@
       <c r="F18" s="40"/>
       <c r="G18" s="37"/>
       <c r="H18" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="42">
         <v>5000000</v>
@@ -2932,23 +3348,23 @@
         <v>6050000</v>
       </c>
       <c r="M18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="N18" s="77"/>
-      <c r="O18" s="78"/>
+        <v>45</v>
+      </c>
+      <c r="N18" s="114"/>
+      <c r="O18" s="115"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A19" s="37">
         <v>3</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="39">
         <v>42033</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
@@ -2956,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I19" s="42">
         <v>1600000</v>
@@ -2971,16 +3387,16 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M19" s="41"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="78"/>
+      <c r="N19" s="114"/>
+      <c r="O19" s="115"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
       <c r="E20" s="45">
         <f>SUM(E17:E19)</f>
         <v>1</v>
@@ -3009,7 +3425,7 @@
       </c>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="1:15" s="6" customFormat="1" ht="15.5">
+    <row r="21" spans="1:15" s="6" customFormat="1" ht="15.75">
       <c r="A21" s="11"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -3024,7 +3440,7 @@
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" ht="18.5">
+    <row r="22" spans="1:15" s="6" customFormat="1" ht="18.75">
       <c r="A22" s="21" t="s">
         <v>1</v>
       </c>
@@ -3037,17 +3453,17 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="80"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="116"/>
+      <c r="L22" s="116"/>
+      <c r="M22" s="117"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:15" s="6" customFormat="1" ht="15.5" hidden="1"/>
-    <row r="25" spans="1:15" s="6" customFormat="1" ht="15.5">
+    <row r="24" spans="1:15" s="6" customFormat="1" ht="15.75" hidden="1"/>
+    <row r="25" spans="1:15" s="6" customFormat="1" ht="15.75">
       <c r="A25" s="24" t="s">
         <v>10</v>
       </c>
@@ -3064,7 +3480,7 @@
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
     </row>
-    <row r="26" spans="1:15" s="6" customFormat="1" ht="15.5">
+    <row r="26" spans="1:15" s="6" customFormat="1" ht="15.75">
       <c r="A26" s="24" t="s">
         <v>11</v>
       </c>
@@ -3075,7 +3491,7 @@
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:15" s="6" customFormat="1" ht="15.5">
+    <row r="27" spans="1:15" s="6" customFormat="1" ht="15.75">
       <c r="A27" s="24" t="s">
         <v>12</v>
       </c>
@@ -3086,7 +3502,7 @@
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="1:15" s="6" customFormat="1" ht="15.5">
+    <row r="28" spans="1:15" s="6" customFormat="1" ht="15.75">
       <c r="A28" s="24" t="s">
         <v>13</v>
       </c>
@@ -3097,15 +3513,15 @@
       <c r="F28" s="22"/>
       <c r="G28" s="25"/>
     </row>
-    <row r="30" spans="1:15" ht="15.5">
+    <row r="30" spans="1:15" ht="15.75">
       <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.5">
+    <row r="31" spans="1:15" ht="15.75">
       <c r="A31" s="26"/>
     </row>
-    <row r="32" spans="1:15" ht="18.5">
+    <row r="32" spans="1:15" ht="18.75">
       <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
@@ -3153,7 +3569,7 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Fix money format
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -1399,6 +1399,63 @@
     <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1416,63 +1473,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2013,9 +2013,7 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
-      <pane xSplit="10" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection activeCell="G12" sqref="G12"/>
-      <selection pane="topRight" activeCell="T22" sqref="T22"/>
+      <selection activeCell="G24" sqref="G24:T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2162,79 +2160,79 @@
       <c r="Y5" s="28"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="107"/>
-      <c r="O6" s="107"/>
-      <c r="P6" s="107"/>
-      <c r="Q6" s="107"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="89"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
+      <c r="Y6" s="89"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
-      <c r="A7" s="107"/>
-      <c r="B7" s="107"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
-      <c r="I7" s="107"/>
-      <c r="J7" s="107"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="107"/>
-      <c r="M7" s="107"/>
-      <c r="N7" s="107"/>
-      <c r="O7" s="107"/>
-      <c r="P7" s="107"/>
-      <c r="Q7" s="107"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+      <c r="P7" s="89"/>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="89"/>
+      <c r="S7" s="89"/>
+      <c r="T7" s="89"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="89"/>
+      <c r="W7" s="89"/>
+      <c r="X7" s="89"/>
+      <c r="Y7" s="89"/>
     </row>
     <row r="8" spans="1:26" ht="19.5">
       <c r="A8" s="8"/>
       <c r="B8" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="98" t="s">
+      <c r="C8" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="98"/>
-      <c r="E8" s="99" t="s">
+      <c r="D8" s="100"/>
+      <c r="E8" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="98" t="s">
+      <c r="F8" s="101"/>
+      <c r="G8" s="100" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -2253,33 +2251,33 @@
       <c r="Y8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="15.75">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="108"/>
-      <c r="N9" s="108"/>
-      <c r="O9" s="108"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="108"/>
-      <c r="R9" s="108"/>
-      <c r="S9" s="108"/>
-      <c r="T9" s="108"/>
-      <c r="U9" s="108"/>
-      <c r="V9" s="108"/>
-      <c r="W9" s="108"/>
-      <c r="X9" s="108"/>
-      <c r="Y9" s="108"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="90"/>
+      <c r="S9" s="90"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="90"/>
+      <c r="X9" s="90"/>
+      <c r="Y9" s="90"/>
     </row>
     <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="47"/>
@@ -2462,83 +2460,83 @@
       <c r="Y15" s="12"/>
     </row>
     <row r="16" spans="1:26" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="E16" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="109" t="s">
+      <c r="F16" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="111"/>
-      <c r="J16" s="95" t="s">
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="95" t="s">
+      <c r="K16" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="95" t="s">
+      <c r="L16" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="M16" s="95" t="s">
+      <c r="M16" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="N16" s="100" t="s">
+      <c r="N16" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="100" t="s">
+      <c r="O16" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="P16" s="100" t="s">
+      <c r="P16" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="Q16" s="112" t="s">
+      <c r="Q16" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="112" t="s">
+      <c r="R16" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="S16" s="112" t="s">
+      <c r="S16" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="T16" s="90" t="s">
+      <c r="T16" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="U16" s="92" t="s">
+      <c r="U16" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="V16" s="93" t="s">
+      <c r="V16" s="112" t="s">
         <v>102</v>
       </c>
-      <c r="W16" s="94" t="s">
+      <c r="W16" s="113" t="s">
         <v>103</v>
       </c>
-      <c r="X16" s="94" t="s">
+      <c r="X16" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="94" t="s">
+      <c r="Y16" s="113" t="s">
         <v>100</v>
       </c>
-      <c r="Z16" s="89"/>
+      <c r="Z16" s="108"/>
     </row>
     <row r="17" spans="1:26" s="5" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A17" s="96"/>
-      <c r="B17" s="101"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="32" t="s">
         <v>21</v>
       </c>
@@ -2551,23 +2549,23 @@
       <c r="I17" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="101"/>
-      <c r="P17" s="101"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="91"/>
-      <c r="U17" s="92"/>
-      <c r="V17" s="93"/>
-      <c r="W17" s="94"/>
-      <c r="X17" s="94"/>
-      <c r="Y17" s="94"/>
-      <c r="Z17" s="89"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="94"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="94"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="110"/>
+      <c r="U17" s="111"/>
+      <c r="V17" s="112"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="113"/>
+      <c r="Y17" s="113"/>
+      <c r="Z17" s="108"/>
     </row>
     <row r="18" spans="1:26" s="5" customFormat="1" ht="15.75">
       <c r="A18" s="70" t="s">
@@ -2787,10 +2785,10 @@
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
-      <c r="I23" s="113" t="s">
+      <c r="I23" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="113"/>
+      <c r="J23" s="107"/>
       <c r="K23" s="23" t="s">
         <v>2</v>
       </c>
@@ -2810,13 +2808,13 @@
       <c r="Y23" s="106"/>
     </row>
     <row r="24" spans="1:26" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A24" s="97" t="s">
+      <c r="A24" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
       <c r="G24" s="105" t="s">
         <v>95</v>
       </c>
@@ -2923,6 +2921,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="G24:T24"/>
+    <mergeCell ref="L23:Y23"/>
+    <mergeCell ref="I23:J23"/>
     <mergeCell ref="A6:Y7"/>
     <mergeCell ref="A9:Y9"/>
     <mergeCell ref="A16:A17"/>
@@ -2939,24 +2955,6 @@
     <mergeCell ref="P16:P17"/>
     <mergeCell ref="J16:J17"/>
     <mergeCell ref="M16:M17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="G24:T24"/>
-    <mergeCell ref="L23:Y23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3224,40 +3222,40 @@
       <c r="B15" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="91" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="109" t="s">
+      <c r="E15" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="110"/>
-      <c r="G15" s="111"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="97"/>
       <c r="H15" s="120" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="95" t="s">
+      <c r="K15" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="95" t="s">
+      <c r="L15" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="95" t="s">
+      <c r="M15" s="91" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
       <c r="A16" s="121"/>
       <c r="B16" s="121"/>
-      <c r="C16" s="96"/>
+      <c r="C16" s="92"/>
       <c r="D16" s="121"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
@@ -3270,10 +3268,10 @@
       </c>
       <c r="H16" s="121"/>
       <c r="I16" s="121"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="96"/>
-      <c r="M16" s="96"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A17" s="37">

</xml_diff>

<commit_message>
Edit template bang ke cuoc van chuyen
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_projects\kepler_workspace\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -209,31 +209,7 @@
     <t>SỐ XE</t>
   </si>
   <si>
-    <t>NGÀY VAN CHUYEN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bằng chữ: </t>
-  </si>
-  <si>
-    <t>KHO NHAN HANG</t>
-  </si>
-  <si>
-    <t>KHO GIAO HANG</t>
-  </si>
-  <si>
-    <t>NOI LAY CONT</t>
-  </si>
-  <si>
-    <t>NOI HA CONT</t>
-  </si>
-  <si>
-    <t>GIA CA</t>
-  </si>
-  <si>
-    <t>CHI HO</t>
-  </si>
-  <si>
-    <t>TRONG  LUONG</t>
   </si>
   <si>
     <t>JOB NO</t>
@@ -442,10 +418,34 @@
     <t>${trans.invoiceTruck}</t>
   </si>
   <si>
-    <t>HOA DON CHI HO</t>
-  </si>
-  <si>
     <t>${trans.invoiceMani}</t>
+  </si>
+  <si>
+    <t>TRỌNG LƯỢNG</t>
+  </si>
+  <si>
+    <t>NƠI LẤY CONT</t>
+  </si>
+  <si>
+    <t>NƠI HẠ CONT</t>
+  </si>
+  <si>
+    <t>CHI HỘ</t>
+  </si>
+  <si>
+    <t>HÓA ĐƠN CHI HỘ</t>
+  </si>
+  <si>
+    <t>ĐƠN GIÁ</t>
+  </si>
+  <si>
+    <t>NGÀY VẬN CHUYỂN</t>
+  </si>
+  <si>
+    <t>KHO NHẬN HÀNG</t>
+  </si>
+  <si>
+    <t>KHO GIAO HKHO GIAO HÀNGANG</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1543,6 +1543,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -2058,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2215,7 +2219,7 @@
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1">
       <c r="A6" s="115" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B6" s="115"/>
       <c r="C6" s="115"/>
@@ -2232,17 +2236,17 @@
       <c r="N6" s="115"/>
       <c r="O6" s="115"/>
       <c r="P6" s="115"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
-      <c r="T6" s="115"/>
-      <c r="U6" s="115"/>
-      <c r="V6" s="115"/>
-      <c r="W6" s="115"/>
-      <c r="X6" s="115"/>
-      <c r="Y6" s="115"/>
-      <c r="Z6" s="115"/>
-      <c r="AA6" s="115"/>
+      <c r="Q6" s="137"/>
+      <c r="R6" s="137"/>
+      <c r="S6" s="137"/>
+      <c r="T6" s="137"/>
+      <c r="U6" s="137"/>
+      <c r="V6" s="137"/>
+      <c r="W6" s="137"/>
+      <c r="X6" s="137"/>
+      <c r="Y6" s="137"/>
+      <c r="Z6" s="137"/>
+      <c r="AA6" s="137"/>
     </row>
     <row r="7" spans="1:28" ht="15" customHeight="1">
       <c r="A7" s="115"/>
@@ -2261,33 +2265,33 @@
       <c r="N7" s="115"/>
       <c r="O7" s="115"/>
       <c r="P7" s="115"/>
-      <c r="Q7" s="115"/>
-      <c r="R7" s="115"/>
-      <c r="S7" s="115"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
-      <c r="W7" s="115"/>
-      <c r="X7" s="115"/>
-      <c r="Y7" s="115"/>
-      <c r="Z7" s="115"/>
-      <c r="AA7" s="115"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="137"/>
+      <c r="S7" s="137"/>
+      <c r="T7" s="137"/>
+      <c r="U7" s="137"/>
+      <c r="V7" s="137"/>
+      <c r="W7" s="137"/>
+      <c r="X7" s="137"/>
+      <c r="Y7" s="137"/>
+      <c r="Z7" s="137"/>
+      <c r="AA7" s="137"/>
     </row>
     <row r="8" spans="1:28">
       <c r="A8" s="58"/>
       <c r="B8" s="61" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C8" s="105" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D8" s="105"/>
       <c r="E8" s="106" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F8" s="106"/>
       <c r="G8" s="105" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H8" s="105"/>
       <c r="I8" s="105"/>
@@ -2312,7 +2316,7 @@
     </row>
     <row r="9" spans="1:28">
       <c r="A9" s="116" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B9" s="116"/>
       <c r="C9" s="116"/>
@@ -2321,25 +2325,25 @@
       <c r="F9" s="116"/>
       <c r="G9" s="116"/>
       <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-      <c r="T9" s="116"/>
-      <c r="U9" s="116"/>
-      <c r="V9" s="116"/>
-      <c r="W9" s="116"/>
-      <c r="X9" s="116"/>
-      <c r="Y9" s="116"/>
-      <c r="Z9" s="116"/>
-      <c r="AA9" s="116"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="136"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="136"/>
+      <c r="M9" s="136"/>
+      <c r="N9" s="136"/>
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
+      <c r="Q9" s="136"/>
+      <c r="R9" s="136"/>
+      <c r="S9" s="136"/>
+      <c r="T9" s="136"/>
+      <c r="U9" s="136"/>
+      <c r="V9" s="136"/>
+      <c r="W9" s="136"/>
+      <c r="X9" s="136"/>
+      <c r="Y9" s="136"/>
+      <c r="Z9" s="136"/>
+      <c r="AA9" s="136"/>
     </row>
     <row r="10" spans="1:28">
       <c r="A10" s="51"/>
@@ -2378,7 +2382,7 @@
       </c>
       <c r="B11" s="63"/>
       <c r="C11" s="44" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D11" s="44"/>
       <c r="F11" s="65"/>
@@ -2410,7 +2414,7 @@
       </c>
       <c r="B12" s="63"/>
       <c r="C12" s="44" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D12" s="44"/>
       <c r="F12" s="66"/>
@@ -2442,7 +2446,7 @@
       </c>
       <c r="B13" s="63"/>
       <c r="C13" s="44" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D13" s="44"/>
       <c r="F13" s="66"/>
@@ -2474,7 +2478,7 @@
       </c>
       <c r="B14" s="63"/>
       <c r="C14" s="44" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D14" s="63"/>
       <c r="E14" s="44"/>
@@ -2482,7 +2486,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="109" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H14" s="109"/>
       <c r="I14" s="109"/>
@@ -2538,16 +2542,16 @@
         <v>0</v>
       </c>
       <c r="B16" s="107" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C16" s="102" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="D16" s="107" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="E16" s="107" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="F16" s="117" t="s">
         <v>20</v>
@@ -2559,55 +2563,55 @@
         <v>51</v>
       </c>
       <c r="K16" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="102" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="102" t="s">
+        <v>114</v>
+      </c>
+      <c r="N16" s="107" t="s">
+        <v>115</v>
+      </c>
+      <c r="O16" s="107" t="s">
+        <v>116</v>
+      </c>
+      <c r="P16" s="107" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q16" s="107" t="s">
+        <v>118</v>
+      </c>
+      <c r="R16" s="120" t="s">
+        <v>119</v>
+      </c>
+      <c r="S16" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="T16" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="102" t="s">
-        <v>62</v>
-      </c>
-      <c r="M16" s="102" t="s">
-        <v>60</v>
-      </c>
-      <c r="N16" s="107" t="s">
-        <v>56</v>
-      </c>
-      <c r="O16" s="107" t="s">
-        <v>57</v>
-      </c>
-      <c r="P16" s="107" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q16" s="107" t="s">
-        <v>121</v>
-      </c>
-      <c r="R16" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="S16" s="120" t="s">
-        <v>98</v>
-      </c>
-      <c r="T16" s="120" t="s">
+      <c r="U16" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="V16" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="U16" s="98" t="s">
-        <v>113</v>
-      </c>
-      <c r="V16" s="100" t="s">
-        <v>105</v>
-      </c>
       <c r="W16" s="101" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="X16" s="101" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="Y16" s="102" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Z16" s="101" t="s">
         <v>29</v>
       </c>
       <c r="AA16" s="101" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="AB16" s="97"/>
     </row>
@@ -2624,7 +2628,7 @@
         <v>22</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I17" s="52" t="s">
         <v>23</v>
@@ -2651,7 +2655,7 @@
     </row>
     <row r="18" spans="1:28" s="69" customFormat="1">
       <c r="A18" s="54" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B18" s="70"/>
       <c r="C18" s="71"/>
@@ -2682,90 +2686,90 @@
     </row>
     <row r="19" spans="1:28" s="69" customFormat="1" ht="44.25" customHeight="1">
       <c r="A19" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="K19" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="L19" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="74" t="s">
+      <c r="M19" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="74" t="s">
+      <c r="N19" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="75" t="s">
+      <c r="O19" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="75" t="s">
+      <c r="P19" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="75" t="s">
-        <v>111</v>
-      </c>
-      <c r="I19" s="76" t="s">
+      <c r="Q19" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="R19" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="74" t="s">
+      <c r="S19" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="T19" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="U19" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="V19" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="W19" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="X19" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y19" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z19" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="L19" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="M19" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="N19" s="74" t="s">
-        <v>81</v>
-      </c>
-      <c r="O19" s="74" t="s">
-        <v>82</v>
-      </c>
-      <c r="P19" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q19" s="77" t="s">
-        <v>122</v>
-      </c>
-      <c r="R19" s="77" t="s">
-        <v>84</v>
-      </c>
-      <c r="S19" s="78" t="s">
-        <v>96</v>
-      </c>
-      <c r="T19" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="U19" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="V19" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="W19" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="X19" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y19" s="96" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z19" s="77" t="s">
-        <v>85</v>
-      </c>
       <c r="AA19" s="79" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:28" s="69" customFormat="1" ht="19.5" customHeight="1">
       <c r="A20" s="54" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B20" s="80"/>
       <c r="C20" s="80"/>
@@ -2813,31 +2817,31 @@
       <c r="N21" s="85"/>
       <c r="O21" s="85"/>
       <c r="P21" s="86" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="Q21" s="86"/>
       <c r="R21" s="86" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="S21" s="49"/>
       <c r="T21" s="49" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="U21" s="49" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="V21" s="50" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="W21" s="86" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="X21" s="87" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="Y21" s="87"/>
       <c r="Z21" s="49" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="AA21" s="54"/>
     </row>
@@ -2882,7 +2886,7 @@
       <c r="G23" s="91"/>
       <c r="H23" s="91"/>
       <c r="I23" s="114" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J23" s="114"/>
       <c r="K23" s="57" t="s">
@@ -2907,14 +2911,14 @@
     </row>
     <row r="24" spans="1:28" ht="20.25" customHeight="1">
       <c r="A24" s="104" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="104"/>
       <c r="C24" s="104"/>
       <c r="D24" s="104"/>
       <c r="E24" s="104"/>
       <c r="G24" s="112" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H24" s="112"/>
       <c r="I24" s="112"/>
@@ -2968,7 +2972,7 @@
     </row>
     <row r="28" spans="1:28">
       <c r="A28" s="93" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B28" s="58"/>
       <c r="C28" s="58"/>
@@ -2982,7 +2986,7 @@
     </row>
     <row r="29" spans="1:28">
       <c r="A29" s="93" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B29" s="58"/>
       <c r="C29" s="58"/>
@@ -3023,8 +3027,7 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A6:AA7"/>
-    <mergeCell ref="A9:AA9"/>
+    <mergeCell ref="A6:P7"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
@@ -3051,6 +3054,7 @@
     <mergeCell ref="L23:AA23"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="AB16:AB17"/>
     <mergeCell ref="U16:U17"/>
     <mergeCell ref="V16:V17"/>

</xml_diff>

<commit_message>
1. Duplicate chi phi 2. Verify nhathau (0015) 3. delete trung trucking service 4. update ngày 5. bang ke cuoc van chuyen 6. Duyet chi - duyet thu 7. chay so thu tu
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="126">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Nang 275 + hạ 275</t>
   </si>
   <si>
-    <t>Tp. Hồ Chí Minh , ngày  30  tháng  1 năm 2015</t>
-  </si>
-  <si>
     <t>F.3</t>
   </si>
   <si>
@@ -446,6 +443,18 @@
   </si>
   <si>
     <t>SỐ HÓA ĐƠN CHI PHÍ NHÀ THẦU</t>
+  </si>
+  <si>
+    <t>Tp. Hồ Chí Minh , ${updateDate}</t>
+  </si>
+  <si>
+    <t>PHÍ KHÁC</t>
+  </si>
+  <si>
+    <t>${trans.otherFee}</t>
+  </si>
+  <si>
+    <t>${otherFeeTotal}</t>
   </si>
 </sst>
 </file>
@@ -934,7 +943,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1145,6 +1154,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="67">
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
@@ -1215,7 +1246,7 @@
     <xf numFmtId="167" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="39" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="145">
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1428,77 +1459,96 @@
     <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="44" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="41" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="41" fillId="26" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="26" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="41" fillId="26" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="44" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="41" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1545,7 +1595,7 @@
     <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="43" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2060,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB56"/>
+  <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="Q12" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17:W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2084,18 +2134,20 @@
     <col min="15" max="15" width="11.7109375" style="56" customWidth="1"/>
     <col min="16" max="17" width="12.42578125" style="56" customWidth="1"/>
     <col min="18" max="18" width="13.140625" style="56" customWidth="1"/>
-    <col min="19" max="26" width="14.42578125" style="56" customWidth="1"/>
-    <col min="27" max="27" width="16.7109375" style="56" customWidth="1"/>
-    <col min="28" max="28" width="18" style="56" customWidth="1"/>
-    <col min="29" max="16384" width="9" style="56"/>
+    <col min="19" max="22" width="14.42578125" style="56" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="56" customWidth="1"/>
+    <col min="24" max="27" width="14.42578125" style="56" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="56" customWidth="1"/>
+    <col min="29" max="29" width="18" style="56" customWidth="1"/>
+    <col min="30" max="16384" width="9" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="AA1" s="57" t="s">
+    <row r="1" spans="1:28">
+      <c r="AB1" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:28">
       <c r="A2" s="58"/>
       <c r="B2" s="58"/>
       <c r="C2" s="58"/>
@@ -2122,11 +2174,12 @@
       <c r="X2" s="58"/>
       <c r="Y2" s="58"/>
       <c r="Z2" s="58"/>
-      <c r="AA2" s="59" t="s">
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="59" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="58"/>
       <c r="B3" s="58"/>
       <c r="C3" s="58"/>
@@ -2153,11 +2206,12 @@
       <c r="X3" s="58"/>
       <c r="Y3" s="58"/>
       <c r="Z3" s="58"/>
-      <c r="AA3" s="59" t="s">
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="58"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
@@ -2184,11 +2238,12 @@
       <c r="X4" s="58"/>
       <c r="Y4" s="58"/>
       <c r="Z4" s="58"/>
-      <c r="AA4" s="59" t="s">
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="A5" s="58"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -2216,26 +2271,27 @@
       <c r="Y5" s="60"/>
       <c r="Z5" s="60"/>
       <c r="AA5" s="60"/>
-    </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1">
-      <c r="A6" s="118" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-      <c r="N6" s="118"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="118"/>
+      <c r="AB5" s="60"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" customHeight="1">
+      <c r="A6" s="107" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
       <c r="Q6" s="97"/>
       <c r="R6" s="97"/>
       <c r="S6" s="97"/>
@@ -2247,24 +2303,25 @@
       <c r="Y6" s="97"/>
       <c r="Z6" s="97"/>
       <c r="AA6" s="97"/>
-    </row>
-    <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="118"/>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="118"/>
-      <c r="M7" s="118"/>
-      <c r="N7" s="118"/>
-      <c r="O7" s="118"/>
-      <c r="P7" s="118"/>
+      <c r="AB6" s="97"/>
+    </row>
+    <row r="7" spans="1:28" ht="15" customHeight="1">
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
       <c r="Q7" s="97"/>
       <c r="R7" s="97"/>
       <c r="S7" s="97"/>
@@ -2276,29 +2333,30 @@
       <c r="Y7" s="97"/>
       <c r="Z7" s="97"/>
       <c r="AA7" s="97"/>
-    </row>
-    <row r="8" spans="1:27" ht="15" customHeight="1">
+      <c r="AB7" s="97"/>
+    </row>
+    <row r="8" spans="1:28" ht="15" customHeight="1">
       <c r="A8" s="95"/>
       <c r="B8" s="95"/>
       <c r="C8" s="95"/>
       <c r="D8" s="95"/>
-      <c r="E8" s="107" t="s">
+      <c r="E8" s="115" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="115"/>
+      <c r="G8" s="114" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="114"/>
+      <c r="I8" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="107"/>
-      <c r="G8" s="106" t="s">
+      <c r="J8" s="115"/>
+      <c r="K8" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="106"/>
-      <c r="I8" s="107" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="107"/>
-      <c r="K8" s="106" t="s">
-        <v>86</v>
-      </c>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="102"/>
       <c r="N8" s="95"/>
       <c r="O8" s="95"/>
       <c r="P8" s="95"/>
@@ -2313,19 +2371,20 @@
       <c r="Y8" s="97"/>
       <c r="Z8" s="97"/>
       <c r="AA8" s="97"/>
-    </row>
-    <row r="9" spans="1:27">
+      <c r="AB8" s="97"/>
+    </row>
+    <row r="9" spans="1:28">
       <c r="A9" s="58"/>
-      <c r="E9" s="116" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="116"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
+      <c r="E9" s="122" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
       <c r="M9" s="58"/>
       <c r="N9" s="58"/>
       <c r="O9" s="58"/>
@@ -2340,9 +2399,10 @@
       <c r="X9" s="58"/>
       <c r="Y9" s="58"/>
       <c r="Z9" s="58"/>
-      <c r="AA9" s="59"/>
-    </row>
-    <row r="10" spans="1:27">
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="59"/>
+    </row>
+    <row r="10" spans="1:28">
       <c r="I10" s="96"/>
       <c r="J10" s="96"/>
       <c r="K10" s="96"/>
@@ -2362,8 +2422,9 @@
       <c r="Y10" s="96"/>
       <c r="Z10" s="96"/>
       <c r="AA10" s="96"/>
-    </row>
-    <row r="11" spans="1:27">
+      <c r="AB10" s="96"/>
+    </row>
+    <row r="11" spans="1:28">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -2389,18 +2450,19 @@
       <c r="W11" s="51"/>
       <c r="X11" s="51"/>
       <c r="Y11" s="53"/>
-      <c r="Z11" s="51"/>
-      <c r="AA11" s="61" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" s="63" customFormat="1">
+      <c r="Z11" s="100"/>
+      <c r="AA11" s="51"/>
+      <c r="AB11" s="61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="63" customFormat="1">
       <c r="A12" s="62" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="62"/>
       <c r="C12" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="44"/>
       <c r="F12" s="64"/>
@@ -2425,14 +2487,15 @@
       <c r="Y12" s="66"/>
       <c r="Z12" s="66"/>
       <c r="AA12" s="66"/>
-    </row>
-    <row r="13" spans="1:27" s="63" customFormat="1">
+      <c r="AB12" s="66"/>
+    </row>
+    <row r="13" spans="1:28" s="63" customFormat="1">
       <c r="A13" s="62" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="62"/>
       <c r="C13" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="44"/>
       <c r="F13" s="65"/>
@@ -2457,14 +2520,15 @@
       <c r="Y13" s="65"/>
       <c r="Z13" s="65"/>
       <c r="AA13" s="65"/>
-    </row>
-    <row r="14" spans="1:27" s="63" customFormat="1">
+      <c r="AB13" s="65"/>
+    </row>
+    <row r="14" spans="1:28" s="63" customFormat="1">
       <c r="A14" s="62" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="62"/>
       <c r="C14" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="44"/>
       <c r="F14" s="65"/>
@@ -2489,25 +2553,26 @@
       <c r="Y14" s="65"/>
       <c r="Z14" s="65"/>
       <c r="AA14" s="65"/>
-    </row>
-    <row r="15" spans="1:27" s="63" customFormat="1">
+      <c r="AB14" s="65"/>
+    </row>
+    <row r="15" spans="1:28" s="63" customFormat="1">
       <c r="A15" s="62" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="62"/>
       <c r="C15" s="44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="62"/>
       <c r="E15" s="44"/>
       <c r="F15" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="110" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
+      <c r="G15" s="116" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="116"/>
+      <c r="I15" s="116"/>
       <c r="J15" s="64"/>
       <c r="L15" s="65"/>
       <c r="M15" s="65"/>
@@ -2525,8 +2590,9 @@
       <c r="Y15" s="65"/>
       <c r="Z15" s="65"/>
       <c r="AA15" s="65"/>
-    </row>
-    <row r="16" spans="1:27" s="63" customFormat="1" ht="18.75" customHeight="1">
+      <c r="AB15" s="65"/>
+    </row>
+    <row r="16" spans="1:28" s="63" customFormat="1" ht="18.75" customHeight="1">
       <c r="A16" s="67"/>
       <c r="B16" s="51"/>
       <c r="C16" s="64"/>
@@ -2554,91 +2620,95 @@
       <c r="Y16" s="65"/>
       <c r="Z16" s="65"/>
       <c r="AA16" s="65"/>
-    </row>
-    <row r="17" spans="1:28" s="68" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="103" t="s">
+      <c r="AB16" s="65"/>
+    </row>
+    <row r="17" spans="1:29" s="68" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A17" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="108" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="105" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="110" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="108" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="103" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="108" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="108" t="s">
+      <c r="M17" s="108" t="s">
+        <v>112</v>
+      </c>
+      <c r="N17" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="O17" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="P17" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q17" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="119" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="K17" s="103" t="s">
-        <v>81</v>
-      </c>
-      <c r="L17" s="103" t="s">
-        <v>54</v>
-      </c>
-      <c r="M17" s="103" t="s">
-        <v>113</v>
-      </c>
-      <c r="N17" s="108" t="s">
-        <v>114</v>
-      </c>
-      <c r="O17" s="108" t="s">
-        <v>115</v>
-      </c>
-      <c r="P17" s="108" t="s">
+      <c r="R17" s="123" t="s">
         <v>116</v>
       </c>
-      <c r="Q17" s="108" t="s">
+      <c r="S17" s="123" t="s">
+        <v>89</v>
+      </c>
+      <c r="T17" s="123" t="s">
+        <v>88</v>
+      </c>
+      <c r="U17" s="125" t="s">
+        <v>104</v>
+      </c>
+      <c r="V17" s="144" t="s">
+        <v>96</v>
+      </c>
+      <c r="W17" s="127" t="s">
+        <v>93</v>
+      </c>
+      <c r="X17" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y17" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="R17" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="S17" s="117" t="s">
-        <v>90</v>
-      </c>
-      <c r="T17" s="117" t="s">
-        <v>89</v>
-      </c>
-      <c r="U17" s="99" t="s">
-        <v>105</v>
-      </c>
-      <c r="V17" s="101" t="s">
-        <v>97</v>
-      </c>
-      <c r="W17" s="102" t="s">
-        <v>94</v>
-      </c>
-      <c r="X17" s="102" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y17" s="103" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z17" s="102" t="s">
+      <c r="Z17" s="108" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA17" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="AA17" s="102" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB17" s="98"/>
-    </row>
-    <row r="18" spans="1:28" s="68" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="104"/>
-      <c r="B18" s="109"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
+      <c r="AB17" s="127" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC17" s="124"/>
+    </row>
+    <row r="18" spans="1:29" s="68" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="109"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
       <c r="F18" s="52" t="s">
         <v>21</v>
       </c>
@@ -2646,34 +2716,35 @@
         <v>22</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I18" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="104"/>
-      <c r="K18" s="104"/>
-      <c r="L18" s="104"/>
-      <c r="M18" s="104"/>
-      <c r="N18" s="109"/>
-      <c r="O18" s="109"/>
-      <c r="P18" s="109"/>
-      <c r="Q18" s="109"/>
-      <c r="R18" s="117"/>
-      <c r="S18" s="117"/>
-      <c r="T18" s="117"/>
-      <c r="U18" s="100"/>
-      <c r="V18" s="101"/>
-      <c r="W18" s="102"/>
-      <c r="X18" s="102"/>
-      <c r="Y18" s="104"/>
-      <c r="Z18" s="102"/>
-      <c r="AA18" s="102"/>
-      <c r="AB18" s="98"/>
-    </row>
-    <row r="19" spans="1:28" s="68" customFormat="1">
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="106"/>
+      <c r="Q18" s="106"/>
+      <c r="R18" s="123"/>
+      <c r="S18" s="123"/>
+      <c r="T18" s="123"/>
+      <c r="U18" s="126"/>
+      <c r="V18" s="144"/>
+      <c r="W18" s="127"/>
+      <c r="X18" s="127"/>
+      <c r="Y18" s="109"/>
+      <c r="Z18" s="109"/>
+      <c r="AA18" s="127"/>
+      <c r="AB18" s="127"/>
+      <c r="AC18" s="124"/>
+    </row>
+    <row r="19" spans="1:29" s="68" customFormat="1">
       <c r="A19" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="69"/>
       <c r="C19" s="70"/>
@@ -2699,95 +2770,99 @@
       <c r="W19" s="70"/>
       <c r="X19" s="70"/>
       <c r="Y19" s="70"/>
-      <c r="Z19" s="70"/>
+      <c r="Z19" s="98"/>
       <c r="AA19" s="70"/>
-    </row>
-    <row r="20" spans="1:28" s="68" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A20" s="137" t="s">
+      <c r="AB19" s="70"/>
+    </row>
+    <row r="20" spans="1:29" s="68" customFormat="1" ht="44.25" customHeight="1">
+      <c r="A20" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="C20" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="D20" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="E20" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="72" t="s">
+      <c r="F20" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="73" t="s">
+      <c r="G20" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="H20" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="74" t="s">
+      <c r="J20" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="J20" s="72" t="s">
+      <c r="K20" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="72" t="s">
+      <c r="L20" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="L20" s="72" t="s">
+      <c r="M20" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="M20" s="72" t="s">
+      <c r="N20" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="N20" s="72" t="s">
+      <c r="O20" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="O20" s="72" t="s">
+      <c r="P20" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="P20" s="75" t="s">
+      <c r="Q20" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="R20" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="Q20" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="R20" s="75" t="s">
+      <c r="S20" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="T20" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="U20" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="V20" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="W20" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="X20" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y20" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z20" s="103" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA20" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="S20" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="T20" s="75" t="s">
-        <v>91</v>
-      </c>
-      <c r="U20" s="75" t="s">
-        <v>106</v>
-      </c>
-      <c r="V20" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="W20" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="X20" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y20" s="94" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z20" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA20" s="77" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" s="68" customFormat="1" ht="19.5" customHeight="1">
+      <c r="AB20" s="77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" s="68" customFormat="1" ht="19.5" customHeight="1">
       <c r="A21" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
@@ -2813,18 +2888,19 @@
       <c r="W21" s="80"/>
       <c r="X21" s="55"/>
       <c r="Y21" s="55"/>
-      <c r="Z21" s="75"/>
-      <c r="AA21" s="77"/>
-    </row>
-    <row r="22" spans="1:28" ht="19.5" customHeight="1">
-      <c r="A22" s="111" t="s">
+      <c r="Z21" s="55"/>
+      <c r="AA21" s="75"/>
+      <c r="AB21" s="77"/>
+    </row>
+    <row r="22" spans="1:29" ht="19.5" customHeight="1">
+      <c r="A22" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="112"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="112"/>
-      <c r="F22" s="112"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
       <c r="G22" s="81"/>
       <c r="H22" s="81"/>
       <c r="I22" s="81"/>
@@ -2835,35 +2911,38 @@
       <c r="N22" s="83"/>
       <c r="O22" s="83"/>
       <c r="P22" s="84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q22" s="84"/>
       <c r="R22" s="84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S22" s="49"/>
       <c r="T22" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U22" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V22" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="W22" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="W22" s="84" t="s">
-        <v>101</v>
-      </c>
       <c r="X22" s="85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y22" s="85"/>
-      <c r="Z22" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA22" s="54"/>
-    </row>
-    <row r="23" spans="1:28" ht="7.5" customHeight="1">
+      <c r="Z22" s="104" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA22" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB22" s="54"/>
+    </row>
+    <row r="23" spans="1:29" ht="7.5" customHeight="1">
       <c r="A23" s="64"/>
       <c r="B23" s="86"/>
       <c r="C23" s="86"/>
@@ -2889,10 +2968,11 @@
       <c r="W23" s="87"/>
       <c r="X23" s="88"/>
       <c r="Y23" s="88"/>
-      <c r="Z23" s="87"/>
+      <c r="Z23" s="88"/>
       <c r="AA23" s="87"/>
-    </row>
-    <row r="24" spans="1:28">
+      <c r="AB23" s="87"/>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" s="89" t="s">
         <v>1</v>
       </c>
@@ -2903,61 +2983,62 @@
       <c r="F24" s="89"/>
       <c r="G24" s="89"/>
       <c r="H24" s="89"/>
-      <c r="I24" s="115" t="s">
-        <v>107</v>
-      </c>
-      <c r="J24" s="115"/>
+      <c r="I24" s="121" t="s">
+        <v>106</v>
+      </c>
+      <c r="J24" s="121"/>
       <c r="K24" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="114"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="114"/>
-      <c r="P24" s="114"/>
-      <c r="Q24" s="114"/>
-      <c r="R24" s="114"/>
-      <c r="S24" s="114"/>
-      <c r="T24" s="114"/>
-      <c r="U24" s="114"/>
-      <c r="V24" s="114"/>
-      <c r="W24" s="114"/>
-      <c r="X24" s="114"/>
-      <c r="Y24" s="114"/>
-      <c r="Z24" s="114"/>
-      <c r="AA24" s="114"/>
-    </row>
-    <row r="25" spans="1:28" ht="20.25" customHeight="1">
-      <c r="A25" s="105" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="105"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="G25" s="113" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="113"/>
-      <c r="I25" s="113"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="113"/>
-      <c r="L25" s="113"/>
-      <c r="M25" s="113"/>
-      <c r="N25" s="113"/>
-      <c r="O25" s="113"/>
-      <c r="P25" s="113"/>
-      <c r="Q25" s="113"/>
-      <c r="R25" s="113"/>
-      <c r="S25" s="113"/>
-      <c r="T25" s="113"/>
-      <c r="U25" s="113"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="120"/>
+      <c r="R24" s="120"/>
+      <c r="S24" s="120"/>
+      <c r="T24" s="120"/>
+      <c r="U24" s="120"/>
+      <c r="V24" s="120"/>
+      <c r="W24" s="120"/>
+      <c r="X24" s="120"/>
+      <c r="Y24" s="120"/>
+      <c r="Z24" s="120"/>
+      <c r="AA24" s="120"/>
+      <c r="AB24" s="120"/>
+    </row>
+    <row r="25" spans="1:29" ht="20.25" customHeight="1">
+      <c r="A25" s="113" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="G25" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="119"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="119"/>
+      <c r="K25" s="119"/>
+      <c r="L25" s="119"/>
+      <c r="M25" s="119"/>
+      <c r="N25" s="119"/>
+      <c r="O25" s="119"/>
+      <c r="P25" s="119"/>
+      <c r="Q25" s="119"/>
+      <c r="R25" s="119"/>
+      <c r="S25" s="119"/>
+      <c r="T25" s="119"/>
+      <c r="U25" s="119"/>
       <c r="W25" s="47"/>
-      <c r="AA25" s="90"/>
-    </row>
-    <row r="26" spans="1:28" ht="7.5" hidden="1" customHeight="1"/>
-    <row r="27" spans="1:28" ht="7.5" customHeight="1"/>
-    <row r="28" spans="1:28">
+      <c r="AB25" s="90"/>
+    </row>
+    <row r="26" spans="1:29" ht="7.5" hidden="1" customHeight="1"/>
+    <row r="27" spans="1:29" ht="7.5" customHeight="1"/>
+    <row r="28" spans="1:29">
       <c r="A28" s="91" t="s">
         <v>10</v>
       </c>
@@ -2987,10 +3068,11 @@
       <c r="Y28" s="58"/>
       <c r="Z28" s="58"/>
       <c r="AA28" s="58"/>
-    </row>
-    <row r="29" spans="1:28">
+      <c r="AB28" s="58"/>
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29" s="91" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="58"/>
       <c r="C29" s="58"/>
@@ -3002,9 +3084,9 @@
       <c r="I29" s="58"/>
       <c r="J29" s="58"/>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:29">
       <c r="A30" s="91" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="58"/>
       <c r="C30" s="58"/>
@@ -3016,12 +3098,12 @@
       <c r="I30" s="58"/>
       <c r="J30" s="58"/>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:29">
       <c r="A31" s="92"/>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:29">
       <c r="C32" s="47" t="str">
-        <f>AA1</f>
+        <f>AB1</f>
         <v xml:space="preserve">CÔNG TY TNHH THƯƠNG MẠI &amp; DỊCH VỤ AEL </v>
       </c>
       <c r="E32" s="47"/>
@@ -3045,6 +3127,30 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="G25:U25"/>
+    <mergeCell ref="L24:AB24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="E9:L9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="N17:N18"/>
     <mergeCell ref="T17:T18"/>
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="P17:P18"/>
@@ -3058,30 +3164,6 @@
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="M17:M18"/>
     <mergeCell ref="L17:L18"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="G25:U25"/>
-    <mergeCell ref="L24:AA24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="E9:L9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="Y17:Y18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3188,53 +3270,53 @@
       <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="128"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="128"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
-      <c r="K7" s="128"/>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
+      <c r="A7" s="135"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
     </row>
     <row r="8" spans="1:13" ht="15.75">
-      <c r="A8" s="129" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
-      <c r="H8" s="129"/>
-      <c r="I8" s="129"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
+      <c r="A8" s="136" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="136"/>
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="136"/>
     </row>
     <row r="9" spans="1:13" ht="15.75">
       <c r="A9" s="43"/>
@@ -3250,7 +3332,7 @@
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
       <c r="M9" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" ht="15.75">
@@ -3343,47 +3425,47 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="130" t="s">
+      <c r="A15" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="139" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="130" t="s">
+      <c r="D15" s="137" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="134" t="s">
+      <c r="E15" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="135"/>
-      <c r="G15" s="136"/>
-      <c r="H15" s="130" t="s">
+      <c r="F15" s="142"/>
+      <c r="G15" s="143"/>
+      <c r="H15" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="130" t="s">
+      <c r="I15" s="137" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="132" t="s">
+      <c r="J15" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="132" t="s">
+      <c r="K15" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="132" t="s">
+      <c r="L15" s="139" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="132" t="s">
+      <c r="M15" s="139" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="15.75">
-      <c r="A16" s="131"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="131"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="140"/>
+      <c r="D16" s="138"/>
       <c r="E16" s="15" t="s">
         <v>21</v>
       </c>
@@ -3393,12 +3475,12 @@
       <c r="G16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="133"/>
-      <c r="K16" s="133"/>
-      <c r="L16" s="133"/>
-      <c r="M16" s="133"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="140"/>
+      <c r="K16" s="140"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="140"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A17" s="32">
@@ -3434,8 +3516,8 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M17" s="36"/>
-      <c r="N17" s="122"/>
-      <c r="O17" s="123"/>
+      <c r="N17" s="129"/>
+      <c r="O17" s="130"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" ht="33" customHeight="1">
       <c r="A18" s="32">
@@ -3475,15 +3557,15 @@
       <c r="M18" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N18" s="122"/>
-      <c r="O18" s="123"/>
+      <c r="N18" s="129"/>
+      <c r="O18" s="130"/>
     </row>
     <row r="19" spans="1:15" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A19" s="32">
         <v>3</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="34">
         <v>42033</v>
@@ -3497,7 +3579,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="37">
         <v>1600000</v>
@@ -3512,16 +3594,16 @@
         <v>1760000.0000000002</v>
       </c>
       <c r="M19" s="36"/>
-      <c r="N19" s="122"/>
-      <c r="O19" s="123"/>
+      <c r="N19" s="129"/>
+      <c r="O19" s="130"/>
     </row>
     <row r="20" spans="1:15" s="6" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A20" s="124" t="s">
+      <c r="A20" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
       <c r="E20" s="40">
         <f>SUM(E17:E19)</f>
         <v>1</v>
@@ -3578,11 +3660,11 @@
       <c r="H22" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="126"/>
-      <c r="J22" s="126"/>
-      <c r="K22" s="126"/>
-      <c r="L22" s="126"/>
-      <c r="M22" s="127"/>
+      <c r="I22" s="133"/>
+      <c r="J22" s="133"/>
+      <c r="K22" s="133"/>
+      <c r="L22" s="133"/>
+      <c r="M22" s="134"/>
     </row>
     <row r="23" spans="1:15" s="6" customFormat="1" ht="1.5" customHeight="1">
       <c r="M23" s="1"/>

</xml_diff>

<commit_message>
_ fix bug ke toan
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/BangKeCuocVanChuyenTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="3225"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="35" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="126">
   <si>
     <t>SỐ TT</t>
   </si>
@@ -446,7 +451,10 @@
     <t>${otherFeeTotal}</t>
   </si>
   <si>
-    <t>Ref: ${refNo} Tp. Hồ Chí Minh , ${updateDate}</t>
+    <t>Ref: ${refNo}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tp. Hồ Chí Minh , ${updateDate}</t>
   </si>
 </sst>
 </file>
@@ -1470,6 +1478,63 @@
     <xf numFmtId="3" fontId="41" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="41" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1485,65 +1550,8 @@
     <xf numFmtId="167" fontId="41" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="43" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="26" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1858,7 +1866,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1893,7 +1901,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2105,7 +2113,7 @@
   <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2266,24 +2274,24 @@
       <c r="AB5" s="60"/>
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="126"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
       <c r="Q6" s="97"/>
       <c r="R6" s="97"/>
       <c r="S6" s="97"/>
@@ -2298,22 +2306,22 @@
       <c r="AB6" s="97"/>
     </row>
     <row r="7" spans="1:28" ht="15" customHeight="1">
-      <c r="A7" s="126"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
       <c r="Q7" s="97"/>
       <c r="R7" s="97"/>
       <c r="S7" s="97"/>
@@ -2367,18 +2375,20 @@
     </row>
     <row r="9" spans="1:28">
       <c r="A9" s="58"/>
-      <c r="E9" s="124" t="s">
+      <c r="E9" s="122" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
       <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
+      <c r="N9" s="58" t="s">
+        <v>125</v>
+      </c>
       <c r="O9" s="58"/>
       <c r="P9" s="58"/>
       <c r="Q9" s="58"/>
@@ -2558,11 +2568,11 @@
       <c r="F15" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="118" t="s">
+      <c r="G15" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
+      <c r="H15" s="116"/>
+      <c r="I15" s="116"/>
       <c r="J15" s="64"/>
       <c r="L15" s="65"/>
       <c r="M15" s="65"/>
@@ -2613,92 +2623,92 @@
       <c r="AB16" s="65"/>
     </row>
     <row r="17" spans="1:29" s="68" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="116" t="s">
+      <c r="D17" s="105" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="116" t="s">
+      <c r="E17" s="105" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="127" t="s">
+      <c r="F17" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="111" t="s">
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="111" t="s">
+      <c r="K17" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="L17" s="111" t="s">
+      <c r="L17" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="M17" s="111" t="s">
+      <c r="M17" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="N17" s="116" t="s">
+      <c r="N17" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="O17" s="116" t="s">
+      <c r="O17" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="P17" s="116" t="s">
+      <c r="P17" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="Q17" s="116" t="s">
+      <c r="Q17" s="105" t="s">
         <v>119</v>
       </c>
-      <c r="R17" s="125" t="s">
+      <c r="R17" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="S17" s="125" t="s">
+      <c r="S17" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="T17" s="125" t="s">
+      <c r="T17" s="123" t="s">
         <v>87</v>
       </c>
-      <c r="U17" s="106" t="s">
+      <c r="U17" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="V17" s="112" t="s">
+      <c r="V17" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="W17" s="108" t="s">
+      <c r="W17" s="127" t="s">
         <v>92</v>
       </c>
-      <c r="X17" s="108" t="s">
+      <c r="X17" s="127" t="s">
         <v>93</v>
       </c>
-      <c r="Y17" s="109" t="s">
+      <c r="Y17" s="128" t="s">
         <v>120</v>
       </c>
-      <c r="Z17" s="111" t="s">
+      <c r="Z17" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="AA17" s="108" t="s">
+      <c r="AA17" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="AB17" s="108" t="s">
+      <c r="AB17" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="AC17" s="105"/>
+      <c r="AC17" s="124"/>
     </row>
     <row r="18" spans="1:29" s="68" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="110"/>
-      <c r="B18" s="117"/>
-      <c r="C18" s="110"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
       <c r="F18" s="52" t="s">
         <v>21</v>
       </c>
@@ -2711,26 +2721,26 @@
       <c r="I18" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="110"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="110"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="117"/>
-      <c r="P18" s="117"/>
-      <c r="Q18" s="117"/>
-      <c r="R18" s="125"/>
-      <c r="S18" s="125"/>
-      <c r="T18" s="125"/>
-      <c r="U18" s="107"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="108"/>
-      <c r="X18" s="108"/>
-      <c r="Y18" s="110"/>
-      <c r="Z18" s="110"/>
-      <c r="AA18" s="108"/>
-      <c r="AB18" s="108"/>
-      <c r="AC18" s="105"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="106"/>
+      <c r="Q18" s="106"/>
+      <c r="R18" s="123"/>
+      <c r="S18" s="123"/>
+      <c r="T18" s="123"/>
+      <c r="U18" s="126"/>
+      <c r="V18" s="129"/>
+      <c r="W18" s="127"/>
+      <c r="X18" s="127"/>
+      <c r="Y18" s="109"/>
+      <c r="Z18" s="109"/>
+      <c r="AA18" s="127"/>
+      <c r="AB18" s="127"/>
+      <c r="AC18" s="124"/>
     </row>
     <row r="19" spans="1:29" s="68" customFormat="1">
       <c r="A19" s="54" t="s">
@@ -2883,14 +2893,14 @@
       <c r="AB21" s="77"/>
     </row>
     <row r="22" spans="1:29" ht="19.5" customHeight="1">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
       <c r="G22" s="81"/>
       <c r="H22" s="81"/>
       <c r="I22" s="81"/>
@@ -2973,30 +2983,30 @@
       <c r="F24" s="89"/>
       <c r="G24" s="89"/>
       <c r="H24" s="89"/>
-      <c r="I24" s="123" t="s">
+      <c r="I24" s="121" t="s">
         <v>105</v>
       </c>
-      <c r="J24" s="123"/>
+      <c r="J24" s="121"/>
       <c r="K24" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="122"/>
-      <c r="M24" s="122"/>
-      <c r="N24" s="122"/>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="122"/>
-      <c r="V24" s="122"/>
-      <c r="W24" s="122"/>
-      <c r="X24" s="122"/>
-      <c r="Y24" s="122"/>
-      <c r="Z24" s="122"/>
-      <c r="AA24" s="122"/>
-      <c r="AB24" s="122"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="120"/>
+      <c r="R24" s="120"/>
+      <c r="S24" s="120"/>
+      <c r="T24" s="120"/>
+      <c r="U24" s="120"/>
+      <c r="V24" s="120"/>
+      <c r="W24" s="120"/>
+      <c r="X24" s="120"/>
+      <c r="Y24" s="120"/>
+      <c r="Z24" s="120"/>
+      <c r="AA24" s="120"/>
+      <c r="AB24" s="120"/>
     </row>
     <row r="25" spans="1:29" ht="20.25" customHeight="1">
       <c r="A25" s="113" t="s">
@@ -3006,23 +3016,23 @@
       <c r="C25" s="113"/>
       <c r="D25" s="113"/>
       <c r="E25" s="113"/>
-      <c r="G25" s="121" t="s">
+      <c r="G25" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="121"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="121"/>
-      <c r="K25" s="121"/>
-      <c r="L25" s="121"/>
-      <c r="M25" s="121"/>
-      <c r="N25" s="121"/>
-      <c r="O25" s="121"/>
-      <c r="P25" s="121"/>
-      <c r="Q25" s="121"/>
-      <c r="R25" s="121"/>
-      <c r="S25" s="121"/>
-      <c r="T25" s="121"/>
-      <c r="U25" s="121"/>
+      <c r="H25" s="119"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="119"/>
+      <c r="K25" s="119"/>
+      <c r="L25" s="119"/>
+      <c r="M25" s="119"/>
+      <c r="N25" s="119"/>
+      <c r="O25" s="119"/>
+      <c r="P25" s="119"/>
+      <c r="Q25" s="119"/>
+      <c r="R25" s="119"/>
+      <c r="S25" s="119"/>
+      <c r="T25" s="119"/>
+      <c r="U25" s="119"/>
       <c r="W25" s="47"/>
       <c r="AB25" s="90"/>
     </row>
@@ -3117,18 +3127,15 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="A6:P7"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X17:X18"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
@@ -3145,15 +3152,18 @@
     <mergeCell ref="S17:S18"/>
     <mergeCell ref="N17:N18"/>
     <mergeCell ref="T17:T18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="A6:P7"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="L17:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>